<commit_message>
Add product brochures and implement web scraping for product data
</commit_message>
<xml_diff>
--- a/public/LK/lk_ea_products/data/lk_ea_products.xlsx
+++ b/public/LK/lk_ea_products/data/lk_ea_products.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,29 +486,29 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>Image_Path</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Brochure_Path</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Benefits</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>Key_Features</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Benefits</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Image_Path</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Brochure_Path</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/pump-starters-and-controllers/starter/mk-starter</t>
+          <t>https://www.lk-ea.com/products/medium-voltage/air-insulated-switchgear-ais/vh3h</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -538,49 +538,41 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>MK Starter</t>
+          <t>VH3H</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Starter</t>
+          <t>Air Insulated Switchgear Ais</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Since 1960, Lauritz Knudsen Electrical &amp; Automation has been catering to the agriculture, domestic &amp; industrial sectors with a wide range of low motor protection solutions for pumps that help in reliable and efficient irrigation &amp; water management. Our wide range of Direct On-Line (DOL) Starter, Star-Delta Starters, Single Phase &amp; Three Phase variants are the ideal choice for agricultural pumping applications. Available for up to 35 HP pumps, the starters are designed to operate agriculture motors efficiently while offering reliable protection. The 3 phase Starters along with SPPR (single phasing protection relay) provide overload protection, protection from phase unbalance, single phasing, and phase reversal failures. The compact enclosure protects against dust, humidity and insects and is suitable for hot and humid environments. Easy to connect and operate, our Motor Starters are widely acceptable among farmers, industrial owners for individual pumping systems.</t>
+          <t>Our Air Insulated Switchgear offers unparalleled performance up to 36 kV and 50kA, along with a 3-second short circuit withstand capacity, ensuring reliability under intense conditions. With a Loss of Service Continuity-2B rating and IP4X protection, it guarantees uninterrupted operation even in challenging environments. Enhanced with additional customized safety interlocks, this switchgear prioritizes safety without compromising efficiency, demonstrated by its ability to handle numerous operating cycles and maintain optimal performance through efficient 10,000 switching operations. Leveraging our esteemed and validated designs, we've seamlessly integrated cutting-edge connected capabilities, including embedded arc flash protection and health monitoring sensors. At Lauritz Knudsen Electrical &amp; Automation, we believe these advancements empower you to not only optimize the longevity and efficiency of your switchboard but also ensure utmost safety and reliability in your operations.</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Lauritz Knudsen Electrical &amp; Automation began its legacy 70 years ago with the introduction of MK Starters, a cornerstone of reliability in motor control technology. To date, the brand has sold over 25 million units, a testament to the enduring trust and satisfaction of its customers. These starters have been designed to meet the demands of both Direct Online (DOL) and Star-Delta applications, ensuring versatility across a wide range of agricultural and industrial uses. The MK1 and MK2 series are distinguished by their wide-band coil operation, which enhances performance across varied voltage conditions. This feature, coupled with robust design and advanced protective mechanisms, makes MK Starters a preferred choice for ensuring optimal motor efficiency and longevity in demanding agricultural and industrial environments Available Range: MK1 Starters: Relay Range: Up to 13-22 A MK2 Starters: Relay Range: 20-32 A for higher current applications. Direct Online (DOL) Starters: Available up to 7.5hp. Star-Delta Starters: Available up to 15hp. (Offered in fully automatic and semi-automatic configurations)</t>
+          <t>Experience the efficiency and flexibility of VH3H for your power distribution requirements. VH3H is our versatile, globally applicable solution for withdrawable air insulated switchgear, catering to utility, industrial, and infrastructure needs. Its compact design incorporates vacuum circuit breakers, offering a reliable and space-efficient Air-Insulated Switchgear solution at 36 kV.</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Thermal Overload Protection: Highly effective and reliable, ensuring safe operation under various conditions.; Field Proven Starters: Demonstrated reliability and effectiveness in real-world applications.; Wide Band Coil Operation: Capable of operating across a voltage range of 200-400 V.; Reliable Performance in Adverse Conditions: Ensures stable operation in hot, humid environments and under conditions of supply voltage unbalance.; Built-In “ON &amp; OFF” Indication: Provides clear status visibility to operators.; Protective Enclosure: Shields internal components from dust, humidity, and insects.; Compatibility with Voltage/Current Auto SPPR: Ensures seamless integration with safety and performance monitoring systems.; Connection Capability: Can be linked to a Dry Run Protection device to prevent operation under unsafe conditions.</t>
+          <t>images/VH3H.jpg</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Ensures safe operation across various conditions- offers high reliability; Can handle wide range of voltages from 200-400 V.; The design ensures reliable performance in adverse conditions such as hot, humid environments and supply voltage unbalance.; Built-in "ON &amp; OFF" indicators provide clear and immediate operational status to users.; Enhances durability and electrical conductivity for prolonged service life.; Rugged silver-tipped contacts enhance durability and electrical conductivity for prolonged service life.; The protective enclosure shields internal components from dust, humidity, and insects, enhancing longevity.</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>images/MK Starter.jpg</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/Pump_Starter_and_Controller_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>lk_ea_products/brochures/AIS_catalogue.pdf</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/pump-starters-and-controllers/controller/mr-gi-digital-single-phase-controller</t>
+          <t>https://www.lk-ea.com/products/medium-voltage/air-insulated-switchgear-ais/vh1h</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -610,49 +602,41 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>MR-Gi Digital Single Phase Controller</t>
+          <t>VH1H</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Controller</t>
+          <t>Air Insulated Switchgear Ais</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Since 1960, Lauritz Knudsen Electrical &amp; Automation has been integral to Indian agriculture and industry, offering a range of low voltage motor protection solutions. These systems ensure reliable and efficient irrigation and water management, supporting the daily needs of farmers and businesses Designed and developed in-house, our starters and controllers are the preferred choice for efficiently managing pump operations, saving both energy and time for our customers Available for both three-phase and single-phase applications, LK controllers not only protect the motor but also enhance convenience and safety for the user Featuring a robust contactor, Single Phase Preventer, and Dual Voltmeter &amp; Ammeter, this controller offers ease of installation, configuration, and maintenance. Seamlessly integrate it with communicable devices such as the M-POWER+ / M-POWER PRO / M-POWER++ modules for effortless remote pump operation Designed for up to 75 HP pumps in three-phase applications, our controllers efficiently operate agricultural motors and provide reliable protection. They offer overload protection, safeguard against phase unbalance, single phasing, and phase reversal failures, and include an auto-reset feature</t>
+          <t>Our Air Insulated Switchgear offers unparalleled performance up to 36 kV and 50kA, along with a 3-second short circuit withstand capacity, ensuring reliability under intense conditions. With a Loss of Service Continuity-2B rating and IP4X protection, it guarantees uninterrupted operation even in challenging environments. Enhanced with additional customized safety interlocks, this switchgear prioritizes safety without compromising efficiency, demonstrated by its ability to handle numerous operating cycles and maintain optimal performance through efficient 10,000 switching operations. Leveraging our esteemed and validated designs, we've seamlessly integrated cutting-edge connected capabilities, including embedded arc flash protection and health monitoring sensors. At Lauritz Knudsen Electrical &amp; Automation, we believe these advancements empower you to not only optimize the longevity and efficiency of your switchboard but also ensure utmost safety and reliability in your operations.</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>The Digital single-phase controller is offered in three distinct variants to cater to a range of needs: MR-Gi, MR-GiA, and MR-GiB. The MR-Gi model is the manual version, designed for users who prefer control over the basic functions of their system. On the other hand, the MR-GiA and MR-GiB are equipped with automatic functionalities, enhancing convenience and efficiency. The MR-GiA variant is particularly advanced, featuring an in-built Water Level Controller (WLC) that automates water management. In contrast, the MR-GiB does not include a WLC, offering a simpler automatic option for users who do not require this feature. All variants are equipped with an automatic load setting and a digital display that provides critical real-time data on various operational parameters such as voltage and current. This feature allows for better monitoring and management of the controller's performance, ensuring optimal functionality and helping to prevent issues related to electrical parameters. Whether for residential, commercial, or agricultural use, each controller variant is designed to offer tailored solutions, ensuring users have the right tools for efficient management of their single-phase systems. Range Available: ﻿ 0.5 HP to 3 HP (Single Phase Applications Only)</t>
+          <t>Engineered for unparalleled user safety and operational dependability, VH1H is an indoor switchgear assembly that sets a new standard for reliability and performance in the industry. Designed to meet a wide spectrum of electrical distribution requirements up to 12kV, VH1H integrates a suite of pioneering solutions, ensuring utmost reliability and performance.</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Features: MR-Gi Manual version; Microcontroller Based Solution: Ensures precise control and monitoring.; Complete Protection: Guards against dry run, under-voltage, and over-voltage.; Current and Voltage Metering: Allows for detailed monitoring of electrical parameters.; Bypass Mode: Enables manual operation of the system.; Off Timer: Can controls the operational duration.; Digital Display: Provides real-time feedback on system status.; Automatic Current Setting: Adjusts electrical current automatically.; Capacitor Cut-off: Extends the life of capacitors.; Water Tank Status Indication: Indicates water level status to prevent overfill or depletion.</t>
+          <t>images/VH1H.jpg</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Manual mode provides direct control over the system, allowing users to adjust settings based on immediate needs or changes in conditions.; It enables operators to engage directly with the system, offering opportunities for hands-on troubleshooting and fine-tuning.; Automatic mode simplifies operations by managing routine tasks through pre-set controls, reducing the need for constant human intervention.; It enhances consistency in operations by maintaining optimal conditions automatically, minimizing the risk of human error.; Features like the inbuilt Water Level Controller automate water management, ensuring efficient use of resources and prevention of issues such as overflows or dry running.; Timers and delay functions in automatic mode help maintain a schedule, protect equipment, and conserve energy by running the system only when necessary.</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>images/MR-Gi Digital Single Phase Controller.jpg</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/MRGi_Controller_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>lk_ea_products/brochures/IRRD_flyer.pdf</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/pump-starters-and-controllers/solar-solutions/solar-drive-controller</t>
+          <t>https://www.lk-ea.com/products/medium-voltage/ring-main-unit-rmu/fr1-vi</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -682,49 +666,41 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Solar Drive Controller</t>
+          <t>FR1-VI</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Solar Solutions</t>
+          <t>Ring Main Unit Rmu</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Lauritz Knudsen offers cutting-edge solar solutions with its Solar Drive Controller (Px3000), designed to power three-phase Submersible and Monoblock Pumps/Motors for a variety of applications, including irrigation, water supply, farm tank filling, and industrial activities. This robust controller features true MPPT (Maximum Power Point Tracking) to optimise performance even under cloudy conditions, ensuring maximum power extraction from PV panels. It automatically adjusts to changes in current and voltage to maximise output. With its dual supply capability, the Px3000 can operate on both solar and grid power, providing cost savings during daylight hours. Capable of handling input DC voltages up to 850V and operating at temperatures up to 50 degrees Celsius without derating, this controller sets the standard for reliability and efficiency in solar-powered water management</t>
+          <t>Introducing Lauritz Knudsen Electrical &amp; Automation's Ring Main Unit, our innovative SF6 Gas Insulated switchgear, which is a compact, modular, and extendable solution engineered to meet the demands of secondary distribution network switching operations. Featuring six vacuum interrupter-based circuit breakers, this system offers a safe, reliable, and cost-effective option while demanding minimal maintenance. Engineered to withstand formidable conditions of 12kV/17.5kV and 21kA for 3 seconds, its outdoor design prioritizes safety with an intuitive mimic diagram and position indicators for secure operations. Some of the key features include protection against arc faults, live parts isolation ensuring operator safety, passive interlocks to prevent unintended operations, comprehensive padlocking facilities for secure access control, and mimic diagram and position indicators for precise guidance.</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>The Solar Drive Controller (Px3000) offers a robust and intuitive solution tailored to enhance the performance of three-phase submersible and monoblock pump motors across a wide range of applications, including irrigation, water supply, tank filling, and various industrial activities. Featuring advanced true Maximum Power Point Tracking (MPPT) technology, the Px3000 is engineered to optimize the efficiency of solar energy conversion, ensuring that pumps operate at peak performance even under varying solar conditions. Its plug-and-play design simplifies installation, allowing for immediate operation without the need for extensive setup. In addition to its powerful MPPT capability, the Px3000 is adept at functioning in less than ideal solar conditions, such as cloudy weather, ensuring that the maximum possible power is extracted from the photovoltaic (PV) panels at all times. This auto-adjustable feature dynamically alters current and voltage parameters to maximize output, enhancing overall energy efficiency. The dual supply capability of the controller allows it to switch seamlessly between solar and grid power, providing cost-effective operation by leveraging solar power during daylight hours. Furthermore, the controller's ability to operate at temperatures up to 50 degrees Celsius without any derating exemplifies its suitability for challenging environments, ensuring reliable performance regardless of external conditions. Range Available:</t>
+          <t>Introducing Lauritz Knudsen Electrical &amp; Automation's Ring Main Unit, our innovative SF6 Gas Insulated switchgear, which is a compact, modular, and extendable solution engineered to meet the demands of secondary distribution network switching operations. Featuring six vacuum interrupter-based circuit breakers, this system offers a safe, reliable, and cost-effective option while demanding minimal maintenance. Engineered to withstand formidable conditions of 12kV/17.5kV and 21kA for 3 seconds, its outdoor design prioritizes safety with an intuitive mimic diagram and position indicators for secure operations. Some of the key features include protection against arc faults, live parts isolation ensuring operator safety, passive interlocks to prevent unintended operations, comprehensive padlocking facilities for secure access control, and mimic diagram and position indicators for precise guidance.</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>True MPPT Technology: Maximizes water output during the day by optimally converting solar energy into usable power.; Automatic Operation: Automatically starts and stops the pump based on the intensity of sunlight, enhancing energy efficiency.; Dual Energy Compatibility: Operates seamlessly using either solar power or grid electricity, offering flexibility in energy sourcing.; Reverse Polarity Protection: Equipped with a feature that allows the motor to run correctly even if the PV wires are connected to opposite polarity terminals, preventing potential damage.; Plug &amp; Play Installation: Simplifies setup with easy installation; automatically detects and sets necessary parameters like Vmp and Voc without manual input.; Robust Design: Capable of handling very high input DC voltages up to 850V, making it suitable for a wide range of solar applications.</t>
+          <t>images/FR1-VI.jpg</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>True MPPT technology ensures that you get the most efficient use of solar energy throughout the day, maximising water output and reducing energy waste.; The controller's ability to automatically start and stop the pump based on sunlight intensity optimises energy use and prolongs the lifespan of the pump.; Dual energy compatibility provides the flexibility to switch between solar and grid power, ensuring reliable operation regardless of weather conditions and reducing dependency on non-renewable energy sources.; Reverse polarity protection safeguards the motor from installation errors, enhancing the system's reliability and reducing the risk of damage due to incorrect wiring.; The plug and play feature eliminates the need for manual parameter configuration, facilitating quick and easy setup that saves time and minimises setup errors.; A robust design capable of handling high input voltages up to 850V ensures the system can cope with variable solar intensities and maintain stable operation under diverse environmental conditions.</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>images/Solar Drive Controller.jpg</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/Px3000_Solar_Drive_Catalogues.pdf</t>
-        </is>
-      </c>
+          <t>lk_ea_products/brochures/IRRD_flyer.pdf</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/pump-starters-and-controllers/pump-starter-and-controller-spare-accessories/m-power</t>
+          <t>https://www.lk-ea.com/products/medium-voltage/compact-sub-station-css-or-packaged-sub-stations-pss/nqube</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -754,49 +730,41 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>M-POWER</t>
+          <t>NQube</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Pump Starter And Controller Spare Accessories</t>
+          <t>Compact Sub Station Css Or Packaged Sub Stations Pss</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Lauritz Knudsen Electrical &amp; Automation is dedicated to providing top-tier accessories that enhance the functionality and efficiency of your systems. Our range includes innovative mobile modules designed for remote sensing, communication, and device control; specialised water level controllers and the Auto WLC K-Curve MCB, specifically tailored for agricultural pumps; power factor correction capacitors; and the SPPR- Sz5, SDz5, SASDz5 series. Additionally, our micro-controller-based i-Protector ensures effortless operation of pumps, integrating futuristic technology to streamline your operations. Committed to excellent customer service, Lauritz Knudsen guarantees the availability of spare parts for all our products and solutions. For detailed information on our spares and their specifications, please consult the provided price list. This ensures you have all the necessary details at your fingertips to maintain and enhance your equipment's performance efficiently.</t>
+          <t>Compact Sub-station, an integral part of Lauritz Knudsen Electrical &amp; Automation's comprehensive product lineup. Engineered for outdoor applications and adhering to IEC 62271-202 standards, Compact Sub-station serves as a compact MV/LV substation, seamlessly integrating into secondary distribution networks. With Lauritz Knudsen's renowned electrical components at its core, Compact Sub-station ensures maintenance-free operation throughout its entire lifecycle, delivering unparalleled performance and peace of mind for your power distribution needs.</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>M-POWER transforms the way you manage your pump systems by providing advanced remote operational capabilities. This innovative module is designed for use with a mobile starter, enabling users to effortlessly monitor and adjust key parameters such as voltage, current, motor run time, and motor status (On/Off) from anywhere, at any time, using their mobile phones. The intuitive interface allows for easy modification of settings including overvoltage (O/V), under-voltage (U/V), and dry run protection (DRP), enhancing the safety and efficiency of pump operations. Available in three distinct variants—M-POWER++, M-POWER+, and M-POWER Pro—each option is tailored to meet varying needs and preferences. Whether it's for agricultural, residential, commercial, or industrial use, the M-POWER series offers a scalable solution that not only simplifies management but also optimizes performance. These variants ensure that users can select a  mobile starter system that best fits their specific requirements, providing a versatile and reliable approach to pump management and protection.</t>
+          <t>NQube, setting a new benchmark for excellence, is meticulously crafted to meet the standards of IEC 62271-202. It is suitable for LV Switchgear upto 2000A, 440V, Transformer upto 1250kVA and can accommodate 12kV, 630A, 21kA, RMU. Fully factory assembled and type-tested, it guarantees reliability and efficiency from the get-go. Its modular and compartmentalised design allows for easy customisation and maintenance, while the specially designed ventilation system reinforces its durability. With operator safety as a top priority, it provides a completely safe environment for personnel. Additionally, it comes ready for installation and network connection, making deployment swift and hassle-free. Furthermore, its SCADA compatibility and readiness for integration into smart grids position it at the forefront of modern power distribution technologies.</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>M-POWER Pro Features:; Remote Access and Control: Operate your pump from anywhere at any time using SMS, IVRS, calls, and the Lauritz Knudsen Connect Android app for remote ON/OFF, parameter adjustments, monitoring, and troubleshooting.; Simple Installation: Features a 3-wire connection compatible with both Direct On Line (DOL) and Star Delta starters, ensuring easy setup.; Comprehensive Protection: Provides safeguards against phase loss, voltage imbalance, phase reversal, over-voltage, and under-voltage, along with a dry run fault; each protection mechanism can be individually enabled or disabled.; Versatile Compatibility: Compatible with three-phase DOL and Star Delta starters.; Advanced Timing Functions: Includes hour-based and network-based daily timers with four time slots and time compensation features.; Multi-User Control: Allows up to four users and one master to control the pump starter/controller via mobile phones.; Operational Flexibility: Offers auto, manual, and bypass modes and displays total run time information for your pump.; App Integration: Parameters like pump status (ON/OFF) and metering can be easily set and checked through the Lauritz Knudsen Connect App.; M-POWER++ / M-POWER+ Features:</t>
+          <t>images/NQube.jpg</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Remote Accessibility and Control: Users can operate their pump systems from any location at any time, ensuring full control over operations via a mobile app, which enhances flexibility and responsiveness to system needs.; Easy Installation and Versatile Use: The system's three-wire setup simplifies installation processes, and its compatibility with both DOL and Star Delta mobile starter makes it suitable for a wide range of applications, reducing setup time and complexity.; Comprehensive Safety Measures: M-Power Pro provides robust protection against electrical faults such as phase loss, voltage imbalances, and power surges, ensuring the longevity and reliability of pump operations.; Enhanced Operational Efficiency: Features like multi-user control, advanced timing functions, and operational flexibility via auto, manual, and bypass modes allow for precise management of run times and system monitoring, improving overall efficiency and productivity.; Communicative Interaction and Support: With support for multiple languages and the ability to receive real-time updates and notifications via SMS, users can stay informed about their system’s status and make timely decisions based on accurate operational data.; Preventive Maintenance and Protection: The inclusion of an hour meter helps in planning preventive maintenance, while adjustable ON delay timers offer added protection against mechanical stress caused by water hammer, extending the system's lifespan and ensuring continuous operation.</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>images/M-POWER.jpg</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/Pump_Starter_and_Controller_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>lk_ea_products/brochures/NQube_Flyer.pdf</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/medium-voltage/air-insulated-switchgear-ais/vh3h</t>
+          <t>https://www.lk-ea.com/products/medium-voltage/vacuum-circuit-breaker-vcb/vk-series</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -826,41 +794,41 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>VH3H</t>
+          <t>VK Series</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Air Insulated Switchgear Ais</t>
+          <t>Vacuum Circuit Breaker Vcb</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Our Air Insulated Switchgear offers unparalleled performance up to 36 kV and 50kA, along with a 3-second short circuit withstand capacity, ensuring reliability under intense conditions. With a Loss of Service Continuity-2B rating and IP4X protection, it guarantees uninterrupted operation even in challenging environments. Enhanced with additional customized safety interlocks, this switchgear prioritizes safety without compromising efficiency, demonstrated by its ability to handle numerous operating cycles and maintain optimal performance through efficient 10,000 switching operations. Leveraging our esteemed and validated designs, we've seamlessly integrated cutting-edge connected capabilities, including embedded arc flash protection and health monitoring sensors. At Lauritz Knudsen Electrical &amp; Automation, we believe these advancements empower you to not only optimize the longevity and efficiency of your switchboard but also ensure utmost safety and reliability in your operations.</t>
+          <t>With offerings up to 33kV, our 'draw out' type VCBs provide unparalleled convenience and safety, allowing for direct racking out on the floor. Our VCBs are quite dependable and are used across varied Sector.</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Experience the efficiency and flexibility of VH3H for your power distribution requirements. VH3H is our versatile, globally applicable solution for withdrawable air insulated switchgear, catering to utility, industrial, and infrastructure needs. Its compact design incorporates vacuum circuit breakers, offering a reliable and space-efficient Air-Insulated Switchgear solution at 36 kV.</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>images/VH3H.jpg</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/AIS_catalogue.pdf</t>
-        </is>
-      </c>
+          <t>The VK Series VCBs are engineered to operate efficiently and prioritise user safety, drawing from years of experience. They are available up to 12kV with a short circuit breaking capacity of 50kA, reflecting their robust design and innovative approach.</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>images/VK Series.jpg</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>lk_ea_products/brochures/IRRD_flyer.pdf</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/medium-voltage/air-insulated-switchgear-ais/vh1h</t>
+          <t>https://www.lk-ea.com/products/lv-iec-panels/pcc-and-mcc-panels/enersys</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -890,41 +858,41 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>VH1H</t>
+          <t>Enersys</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Air Insulated Switchgear Ais</t>
+          <t>Pcc And Mcc Panels</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Our Air Insulated Switchgear offers unparalleled performance up to 36 kV and 50kA, along with a 3-second short circuit withstand capacity, ensuring reliability under intense conditions. With a Loss of Service Continuity-2B rating and IP4X protection, it guarantees uninterrupted operation even in challenging environments. Enhanced with additional customized safety interlocks, this switchgear prioritizes safety without compromising efficiency, demonstrated by its ability to handle numerous operating cycles and maintain optimal performance through efficient 10,000 switching operations. Leveraging our esteemed and validated designs, we've seamlessly integrated cutting-edge connected capabilities, including embedded arc flash protection and health monitoring sensors. At Lauritz Knudsen Electrical &amp; Automation, we believe these advancements empower you to not only optimize the longevity and efficiency of your switchboard but also ensure utmost safety and reliability in your operations.</t>
+          <t>Lauritz Knudsen is a leader in low-voltage electrical switchboards, delivering IEC-certified solutions that blend technical expertise, safety, and innovation. Built to meet global standards, Lauritz Knudsen switchboards are essential to modern &amp; digital electrical distribution systems, ensuring reliable power flow across factories, infrastructure, and specialized industrial applications. Each unit is engineered for optimal performance, offering safe switching, metering, and circuit protection, with the flexibility to be customized for diverse operational needs. Featuring robust enclosures and precision-built components, Lauritz Knudsen switchboards enable efficient energy management, helping facilities operate with greater confidence, control, digitalization and sustainability.</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Engineered for unparalleled user safety and operational dependability, VH1H is an indoor switchgear assembly that sets a new standard for reliability and performance in the industry. Designed to meet a wide spectrum of electrical distribution requirements up to 12kV, VH1H integrates a suite of pioneering solutions, ensuring utmost reliability and performance.</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>images/VH1H.jpg</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/IRRD_flyer.pdf</t>
-        </is>
-      </c>
+          <t>Enersys by Lauritz Knudsen Electrical &amp; Automation is more than a power distribution unit—it's a blend of smart engineering and digital innovation. Crafted for superior safety, reliability, and efficiency, it combines advanced technology with a sleek, modern look, ensuring your electrical systems are secure and future-proof. Enersys, a true smart panel, integrates advanced communication capabilities, intelligent thermal management, and eco-conscious engineering design for next-generation power solutions. Backed by Lauritz Knudsen Electrical &amp; Automation’s 70-year legacy of powering India, it delivers reliable, future-ready electrical systems tailored for Indian conditions, blending performance with innovation.</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>images/Enersys.jpg</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>lk_ea_products/brochures/Enersys.pdf</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/medium-voltage/ring-main-unit-rmu/fr1-vi</t>
+          <t>https://www.lk-ea.com/products/lv-iec-panels/pcc-and-mcc-panels/ti</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -954,41 +922,41 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>FR1-VI</t>
+          <t>Ti</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Ring Main Unit Rmu</t>
+          <t>Pcc And Mcc Panels</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Introducing Lauritz Knudsen Electrical &amp; Automation's Ring Main Unit, our innovative SF6 Gas Insulated switchgear, which is a compact, modular, and extendable solution engineered to meet the demands of secondary distribution network switching operations. Featuring six vacuum interrupter-based circuit breakers, this system offers a safe, reliable, and cost-effective option while demanding minimal maintenance. Engineered to withstand formidable conditions of 12kV/17.5kV and 21kA for 3 seconds, its outdoor design prioritizes safety with an intuitive mimic diagram and position indicators for secure operations. Some of the key features include protection against arc faults, live parts isolation ensuring operator safety, passive interlocks to prevent unintended operations, comprehensive padlocking facilities for secure access control, and mimic diagram and position indicators for precise guidance.</t>
+          <t>Lauritz Knudsen is a leader in low-voltage electrical switchboards, delivering IEC-certified solutions that blend technical expertise, safety, and innovation. Built to meet global standards, Lauritz Knudsen switchboards are essential to modern &amp; digital electrical distribution systems, ensuring reliable power flow across factories, infrastructure, and specialized industrial applications. Each unit is engineered for optimal performance, offering safe switching, metering, and circuit protection, with the flexibility to be customized for diverse operational needs. Featuring robust enclosures and precision-built components, Lauritz Knudsen switchboards enable efficient energy management, helping facilities operate with greater confidence, control, digitalization and sustainability.</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Introducing Lauritz Knudsen Electrical &amp; Automation's Ring Main Unit, our innovative SF6 Gas Insulated switchgear, which is a compact, modular, and extendable solution engineered to meet the demands of secondary distribution network switching operations. Featuring six vacuum interrupter-based circuit breakers, this system offers a safe, reliable, and cost-effective option while demanding minimal maintenance. Engineered to withstand formidable conditions of 12kV/17.5kV and 21kA for 3 seconds, its outdoor design prioritizes safety with an intuitive mimic diagram and position indicators for secure operations. Some of the key features include protection against arc faults, live parts isolation ensuring operator safety, passive interlocks to prevent unintended operations, comprehensive padlocking facilities for secure access control, and mimic diagram and position indicators for precise guidance.</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>images/FR1-VI.jpg</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/IRRD_flyer.pdf</t>
-        </is>
-      </c>
+          <t>Ti by Lauritz Knudsen Electrical &amp; Automation, a fully type – tested CDV (Complete Design Verified assembly) designed in accordance with the latest IEC 61439 1&amp;2, offering a cutting-edge switchboard solution that embodies legacy of excellence in catering to Indian customers. Ti, Lauritz Knudsen Electrical and automation’s Deming Prize – winning TQM standards, which are evident in every aspect of Ti’s design, manufacture, and quality control. Ti also features state – of – the – art digitalization for remote monitoring and management and employs sustainable materials for environmental care.</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>images/Ti.jpg</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>lk_ea_products/brochures/Ti_Catalogue_-_Final_Dec_2025.pdf</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/medium-voltage/compact-sub-station-css-or-packaged-sub-stations-pss/nqube</t>
+          <t>https://www.lk-ea.com/products/lv-iec-panels/sub-main-distribution-board-smdb/enersys-s</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1018,41 +986,45 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>NQube</t>
+          <t>Enersys S</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Compact Sub Station Css Or Packaged Sub Stations Pss</t>
+          <t>Sub Main Distribution Board Smdb</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Compact Sub-station, an integral part of Lauritz Knudsen Electrical &amp; Automation's comprehensive product lineup. Engineered for outdoor applications and adhering to IEC 62271-202 standards, Compact Sub-station serves as a compact MV/LV substation, seamlessly integrating into secondary distribution networks. With Lauritz Knudsen's renowned electrical components at its core, Compact Sub-station ensures maintenance-free operation throughout its entire lifecycle, delivering unparalleled performance and peace of mind for your power distribution needs.</t>
+          <t>SMDB from Lauritz Knudsen Electrical and automation meet the demands of commercial buildings, educational establishments, hospitals, government buildings, manufacturing facilities and other applications that require safe, reliable &amp; high performance protection of their electrical sub-distribution systems</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>NQube, setting a new benchmark for excellence, is meticulously crafted to meet the standards of IEC 62271-202. It is suitable for LV Switchgear upto 2000A, 440V, Transformer upto 1250kVA and can accommodate 12kV, 630A, 21kA, RMU. Fully factory assembled and type-tested, it guarantees reliability and efficiency from the get-go. Its modular and compartmentalised design allows for easy customisation and maintenance, while the specially designed ventilation system reinforces its durability. With operator safety as a top priority, it provides a completely safe environment for personnel. Additionally, it comes ready for installation and network connection, making deployment swift and hassle-free. Furthermore, its SCADA compatibility and readiness for integration into smart grids position it at the forefront of modern power distribution technologies.</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+          <t>Enersys-S Power Distribution board from Lauritz Knudsen Electrical and automation meet the demands of commercial buildings, educational establishments, hospitals, government buildings, manufacturing facilities and other applications that require safe, reliable &amp; high performance protection of their electrical sub-distribution systems Enersys-S is a NABL tested Sub-Main Distribution Board used for power distribution. It has MCCB as incoming and outgoing switching-cum-protection devices. compact MCCB design ensures maximum cabling area within the enclosure Removable top and bottom glad plates are provided for ease of installation &amp; cabling.</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>images/Enersys S.jpg</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>lk_ea_products/brochures/Enersys_S_SMDB_catalogue.pdf</t>
+        </is>
+      </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>images/NQube.jpg</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/NQube_Flyer.pdf</t>
-        </is>
-      </c>
+          <t>Compact solution - Enersys-S saves almost 30% of floor space over conventional panels due to its compact PN system &amp; MCCB's; Protection from risk of shock - Separate earthing for enclosure ensure operator safety; Ease of termination - Enersys-S facilitates separate earth and neutral bars on both the sides with the required number of cable termination points; Off the shelf assembly - Enersys-S is a ready-to-use solution for nay power distribution needs</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/medium-voltage/vacuum-circuit-breaker-vcb/vk-series</t>
+          <t>https://www.lk-ea.com/products/power-distribution-products-lv-switchgear/air-circuit-breaker-acb/u-power-omega</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1067,7 +1039,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Downloaded</t>
+          <t>Not Found on Category Page</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1082,41 +1054,37 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>VK Series</t>
+          <t>U-Power Omega</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Vacuum Circuit Breaker Vcb</t>
+          <t>Air Circuit Breaker Acb</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>With offerings up to 33kV, our 'draw out' type VCBs provide unparalleled convenience and safety, allowing for direct racking out on the floor. Our VCBs are quite dependable and are used across varied Sector.</t>
+          <t>Designed to protect electrical systems from damage due to excessive current caused by overloads, short circuits, and ground faults; Lauritz Knudsen Electrical &amp; Automation are a leading manufacturer of Low Voltage Switchgear for over 50 years. Lauritz Knudsen Electrical &amp; Automation’s Air Circuit Breakers are ideal for high-power applications in low-voltage distribution networks, offering reliability and compactness while meeting the needs of various industries.</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>The VK Series VCBs are engineered to operate efficiently and prioritise user safety, drawing from years of experience. They are available up to 12kV with a short circuit breaking capacity of 50kA, reflecting their robust design and innovative approach.</t>
+          <t>Electrical protection is crucial for ensuring the safety and reliability of power systems. Electrical installations and equipment are susceptible to internal and external faults that can cause severe damage. Circuit Breakers are essential to detect and isolate faults promptly by early detection and localization of faults. Circuit Breakers also aim to minimize the fault duration and isolate faulty parts from the circuit. Electrical systems may experience excessive current caused by overloads, short circuits, and ground faults condition. Lauritz Knudsen Electrical &amp; Automation is a leading manufacturer of Low Voltage Switchgear for over 70 years. Lauritz Knudsen Electrical &amp; Automation’s OMEGA Air Circuit Breakers are ideal for high-power applications in low-voltage distribution networks, offering reliability and compactness &amp; versatility while meeting the needs of various industries.</t>
         </is>
       </c>
       <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>images/VK Series.jpg</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/IRRD_flyer.pdf</t>
-        </is>
-      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>lk_ea_products/brochures/Solar_Catalogue.pdf</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/lv-iec-panels/pcc-and-mcc-panels/ti</t>
+          <t>https://www.lk-ea.com/products/power-distribution-products-lv-switchgear/air-circuit-breaker-acb/c-power</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1131,7 +1099,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Downloaded</t>
+          <t>Not Found on Category Page</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1146,41 +1114,41 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Ti</t>
+          <t>C-Power</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Pcc And Mcc Panels</t>
+          <t>Air Circuit Breaker Acb</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>We specialise in delivering a wide range of custom-built IEC compliant switchboards that are trusted across diverse industries for their proven reliability. Our product family adheres to international standards, meeting stringent safety and reliability requirements. We take immense pride in offering innovative, future-proof extensive range tailored to meet highest efficiency with customer delight.</t>
+          <t>Designed to protect electrical systems from damage due to excessive current caused by overloads, short circuits, and ground faults; Lauritz Knudsen Electrical &amp; Automation are a leading manufacturer of Low Voltage Switchgear for over 50 years. Lauritz Knudsen Electrical &amp; Automation’s Air Circuit Breakers are ideal for high-power applications in low-voltage distribution networks, offering reliability and compactness while meeting the needs of various industries.</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Ti by Lauritz Knudsen Electrical &amp; Automation, a fully type – tested CDV (Complete Design Verified assembly) designed in accordance with the latest IEC 61439 1&amp;2, offering a cutting-edge switchboard solution that embodies legacy of excellence in catering to Indian customers. Ti, Lauritz Knudsen Electrical and automation’s Deming Prize – winning TQM standards, which are evident in every aspect of Ti’s design, manufacture, and quality control. Ti also features state – of – the – art digitalization for remote monitoring and management and employs sustainable materials for environmental care.</t>
+          <t>Lauritz Knudsen Electrical &amp; Automation offers C-Power range of Air Circuit Breakers (ACBs) up to 6300A, 100kA @415V, designed to safeguard electrical systems from overcurrent and short-circuit faults. C-Power ACBs are tailored to meet all power distribution system requirements, ensuring safe and efficient operation. With a modular design and standardized range, these ACBs are suitable for diverse electrical applications in Buildings, Infrastructure, Utilities and Industries. Special Solution for harsh/corrosive environments is also available in C-Power family</t>
         </is>
       </c>
       <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>lk_ea_products/brochures/C-Power_ACB_Catalogue.pdf</t>
+        </is>
+      </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>images/Ti.jpg</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/Ti_Digital_Brouchure.pdf</t>
-        </is>
-      </c>
+          <t>Leveraging scalability, durability and connectivity, C-Power ACBs integrate technological aspects to enhance uptime and energy efficiency.; Engineered for extreme tropical conditions, these ACBs excel in challenging environments, setting a market benchmark for performance and safety.; With a common door cut-out for the entire range and uniform height and depth for ACBs up to 4000A, they offer flexibility and ease of use.; Entire range offers High Short time withstand capacity, Icu=Ics=Icw for 1 sec to achieve total selectivity and full uptime of system.</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/lv-iec-panels/pcc-and-mcc-panels/enersys</t>
+          <t>https://www.lk-ea.com/products/power-distribution-products-lv-switchgear/moulded-case-circuit-breaker-mccb/dz</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1210,41 +1178,45 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Enersys</t>
+          <t>DZ</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Pcc And Mcc Panels</t>
+          <t>Moulded Case Circuit Breaker Mccb</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>We specialise in delivering a wide range of custom-built IEC compliant switchboards that are trusted across diverse industries for their proven reliability. Our product family adheres to international standards, meeting stringent safety and reliability requirements. We take immense pride in offering innovative, future-proof extensive range tailored to meet highest efficiency with customer delight.</t>
+          <t>The dsine range stands out with its state-of-the-art design, user-friendly features, and a broad spectrum of protection mechanisms, marking it as a leader in the new generation of MCCBs (Moulded Case Circuit Breakers). Recognised for its ergonomic design, aesthetic appeal, and compactness, it is specifically engineered to perform reliably under extreme tropical conditions, offering consistent functionality in high ambient and humid environments. This makes the dsine MCCBs ideal for demanding settings, always meeting the evolving needs of our customers, a testament to our in-depth analysis and responsiveness to customer feedback.</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Enersys by Lauritz Knudsen Electrical &amp; Automation is more than a power distribution unit—it's a blend of smart engineering and digital innovation. Crafted for superior safety, reliability, and efficiency, it combines advanced technology with a sleek, modern look, ensuring your electrical systems are secure and future-proof. Enersys, a true smart panel, integrates advanced communication capabilities, intelligent thermal management, and eco-conscious engineering design for next-generation power solutions. Backed by Lauritz Knudsen Electrical &amp; Automation’s 70-year legacy of powering India, it delivers reliable, future-ready electrical systems tailored for Indian conditions, blending performance with innovation.</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+          <t>The DZ range of Moulded Case Circuit Breakers (MCCB) is specifically designed to accommodate the complexities of modern electrical systems in contemporary installations. This range stands out due to its substantially higher fault-breaking capacities, addressing the rigorous demands of evolving power distribution requirements efficiently and effectively. Responding to the shifting expectations of customers who seek economical yet reliable solutions, we have developed the DZ range of MCCBs that can operate up to 800V AC, with exceptional fault-breaking capacities reaching up to 200kA at 415V AC. Available in both thermal magnetic and electronic versions, these MCCBs provide comprehensive protection, encompassing advanced current, voltage, frequency, power, and harmonic-based safeguards. This versatility empowers system designers and users to select and implement protection schemes that best fit their specific requirements, ensuring tailored and robust electrical safety.</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>images/DZ.jpg</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>lk_ea_products/brochures/Solar_Catalogue.pdf</t>
+        </is>
+      </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>images/Enersys.jpg</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/Enersys.pdf</t>
-        </is>
-      </c>
+          <t>No load line bias ensures balanced power distribution, enhancing system efficiency.; Finger-proof terminals increase safety by preventing accidental contact, crucial for maintaining secure operations.; Phase barriers included with MCCBs enhance safety by effectively preventing electrical arcing between phases.; A wide range of common internal and external accessories is available, offering extensive customisation options to meet specific system requirements.</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/lv-iec-panels/sub-main-distribution-board-smdb/enersys-s</t>
+          <t>https://www.lk-ea.com/products/power-distribution-products-lv-switchgear/moulded-case-circuit-breaker-mccb/dn</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1274,45 +1246,49 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Enersys S</t>
+          <t>DN</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Sub Main Distribution Board Smdb</t>
+          <t>Moulded Case Circuit Breaker Mccb</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>SMDB from Lauritz Knudsen Electrical and automation meet the demands of commercial buildings, educational establishments, hospitals, government buildings, manufacturing facilities and other applications that require safe, reliable &amp; high performance protection of their electrical sub-distribution systems</t>
+          <t>The dsine range stands out with its state-of-the-art design, user-friendly features, and a broad spectrum of protection mechanisms, marking it as a leader in the new generation of MCCBs (Moulded Case Circuit Breakers). Recognised for its ergonomic design, aesthetic appeal, and compactness, it is specifically engineered to perform reliably under extreme tropical conditions, offering consistent functionality in high ambient and humid environments. This makes the dsine MCCBs ideal for demanding settings, always meeting the evolving needs of our customers, a testament to our in-depth analysis and responsiveness to customer feedback.</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Enersys-S Power Distribution board from Lauritz Knudsen Electrical and automation meet the demands of commercial buildings, educational establishments, hospitals, government buildings, manufacturing facilities and other applications that require safe, reliable &amp; high performance protection of their electrical sub-distribution systems Enersys-S is a NABL tested Sub-Main Distribution Board used for power distribution. It has MCCB as incoming and outgoing switching-cum-protection devices. compact MCCB design ensures maximum cabling area within the enclosure Removable top and bottom glad plates are provided for ease of installation &amp; cabling.</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr"/>
+          <t>The dsine range stands out with its state-of-the-art design, user-friendly features, and a broad spectrum of protection mechanisms, marking it as a leader in the new generation of MCCBs (Moulded Case Circuit Breakers). Recognised for its ergonomic design, aesthetic appeal, and compactness, it is specifically engineered to perform reliably under extreme tropical conditions, offering consistent functionality in high ambient and humid environments. This makes the dsine MCCBs ideal for demanding settings, always meeting the evolving needs of our customers, a testament to our in-depth analysis and responsiveness to customer feedback. Understanding and anticipating the requirements of our customers, our contemporary range of MCCBs ensures complete customer satisfaction without compromise. Enhanced by a comprehensive selection of accessories, the dsine range provides complete solutions tailored to various customer applications. This integration ensures not only operational safety and reliability but also adds versatility to its use across different industries and systems, making it a robust choice for comprehensive electrical protection.</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>images/DN.jpg</t>
+        </is>
+      </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Compact solution - Enersys-S saves almost 30% of floor space over conventional panels due to its compact PN system &amp; MCCB's; Protection from risk of shock - Separate earthing for enclosure ensure operator safety; Ease of termination - Enersys-S facilitates separate earth and neutral bars on both the sides with the required number of cable termination points; Off the shelf assembly - Enersys-S is a ready-to-use solution for nay power distribution needs</t>
+          <t>lk_ea_products/brochures/dSine_MCCB_Catalogue.pdf</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>images/Enersys S.jpg</t>
+          <t>No load line bias ensures balanced power distribution without preferential pathways.; Finger-proof terminals enhance safety by preventing accidental contact.; Suitable for DC applications, offering versatility across different electrical setups.; Phase barriers are provided with MCCBs to enhance safety by preventing electrical arcing between phases.; A wide range of common internal and external accessories is available, enabling easy integration and customisation to meet specific system requirements.</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>lk_ea_products/brochures/Enersys_S_SMDB_catalogue.pdf</t>
+          <t>Breaking Capacity: Options available at 25kA, 36kA, 50kA, 70kA, and 100kA, ensuring robust protection against high fault levels.; Variants: Choose from 3-pole or 4-pole versions to suit different circuit configurations.; Compliance: Fully compliant with IEC60947-2, EN60947-2, and IS/IEC60947-2 standards, ensuring international quality and safety benchmarks.; Protection Releases: Features both thermal-magnetic and microprocessor-based protection releases, offering precise and reliable circuit protection.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/power-distribution-products/air-circuit-breaker-acb/u-power-omega</t>
+          <t>https://www.lk-ea.com/products/power-distribution-products-lv-switchgear/moulded-case-circuit-breaker-mccb/dy</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1327,7 +1303,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Not Found on Category Page</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1342,37 +1318,45 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>U-Power Omega</t>
+          <t>DY</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Air Circuit Breaker Acb</t>
+          <t>Moulded Case Circuit Breaker Mccb</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Designed to protect electrical systems from damage due to excessive current caused by overloads, short circuits, and ground faults; Lauritz Knudsen Electrical &amp; Automation are a leading manufacturer of Low Voltage Switchgear for over 50 years. Lauritz Knudsen Electrical &amp; Automation’s Air Circuit Breakers are ideal for high-power applications in low-voltage distribution networks, offering reliability and compactness while meeting the needs of various industries.</t>
+          <t>The dsine range stands out with its state-of-the-art design, user-friendly features, and a broad spectrum of protection mechanisms, marking it as a leader in the new generation of MCCBs (Moulded Case Circuit Breakers). Recognised for its ergonomic design, aesthetic appeal, and compactness, it is specifically engineered to perform reliably under extreme tropical conditions, offering consistent functionality in high ambient and humid environments. This makes the dsine MCCBs ideal for demanding settings, always meeting the evolving needs of our customers, a testament to our in-depth analysis and responsiveness to customer feedback.</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Electrical protection is crucial for ensuring the safety and reliability of power systems. Electrical installations and equipment are susceptible to internal and external faults that can cause severe damage. Circuit Breakers are essential to detect and isolate faults promptly by early detection and localization of faults. Circuit Breakers also aim to minimize the fault duration and isolate faulty parts from the circuit. Electrical systems may experience excessive current caused by overloads, short circuits, and ground faults condition. Lauritz Knudsen Electrical &amp; Automation is a leading manufacturer of Low Voltage Switchgear for over 70 years. Lauritz Knudsen Electrical &amp; Automation’s OMEGA Air Circuit Breakers are ideal for high-power applications in low-voltage distribution networks, offering reliability and compactness &amp; versatility while meeting the needs of various industries.</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/LK_U-Power_OMEGA_Technical_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>The DY Series represents the next generation of MCCBs, distinguished by its state-of-the-art design that combines contemporary, user-friendly features with outstanding ergonomics, aesthetics, and compactness. This series excels in functionality and form, making it an ideal choice for modern electrical infrastructure needs. In terms of compliance, the DY Series adheres to the latest international standards including IS/IEC 60947-2, IEC 60947-2, and EN 60947-2. Each product in the range carries the CE marking, affirming its quality and safety for use even in humid environments. Furthermore, equipped with a wide array of accessories, the series ensures operational safety, reliability, and versatility, meeting even the most demanding system requirements.</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>images/DY.jpg</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>lk_ea_products/brochures/DU_DY_MCCB_Catalogue.pdf</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>The design is compact, optimising space and simplifying installation processes.; No load line bias ensures balanced power distribution, enhancing system efficiency.; Finger-proof terminals increase safety by preventing accidental contact, crucial in maintaining secure operations.; Phase barriers included with MCCBs enhance safety by effectively preventing electrical arcing between phases.</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/power-distribution-products/air-circuit-breaker-acb/c-power</t>
+          <t>https://www.lk-ea.com/products/power-distribution-products-lv-switchgear/moulded-case-circuit-breaker-mccb/du</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1387,7 +1371,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Not Found on Category Page</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1402,41 +1386,45 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>C-Power</t>
+          <t>DU</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Air Circuit Breaker Acb</t>
+          <t>Moulded Case Circuit Breaker Mccb</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Designed to protect electrical systems from damage due to excessive current caused by overloads, short circuits, and ground faults; Lauritz Knudsen Electrical &amp; Automation are a leading manufacturer of Low Voltage Switchgear for over 50 years. Lauritz Knudsen Electrical &amp; Automation’s Air Circuit Breakers are ideal for high-power applications in low-voltage distribution networks, offering reliability and compactness while meeting the needs of various industries.</t>
+          <t>The dsine range stands out with its state-of-the-art design, user-friendly features, and a broad spectrum of protection mechanisms, marking it as a leader in the new generation of MCCBs (Moulded Case Circuit Breakers). Recognised for its ergonomic design, aesthetic appeal, and compactness, it is specifically engineered to perform reliably under extreme tropical conditions, offering consistent functionality in high ambient and humid environments. This makes the dsine MCCBs ideal for demanding settings, always meeting the evolving needs of our customers, a testament to our in-depth analysis and responsiveness to customer feedback.</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Lauritz Knudsen Electrical &amp; Automation offers C-Power range of Air Circuit Breakers (ACBs) up to 6300A, 100kA @415V, designed to safeguard electrical systems from overcurrent and short-circuit faults. C-Power ACBs are tailored to meet all power distribution system requirements, ensuring safe and efficient operation. With a modular design and standardized range, these ACBs are suitable for diverse electrical applications in Buildings, Infrastructure, Utilities and Industries. Special Solution for harsh/corrosive environments is also available in C-Power family</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr"/>
+          <t>The DU Series represents the next generation of MCCBs, distinguished by its state-of-the-art design that combines contemporary, user-friendly features with outstanding ergonomics, aesthetics, and compactness. This series excels in functionality and form, making it an ideal choice for modern electrical infrastructure needs. In terms of compliance, the DU Series adheres to the latest international standards including IS/IEC 60947-2, IEC 60947-2, and EN 60947-2. Each product in the range carries the CE marking, affirming its quality and safety for use even in humid environments. Furthermore, equipped with a wide array of accessories, the series ensures operational safety, reliability, and versatility, meeting even the most demanding system requirements.</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>images/DU.jpg</t>
+        </is>
+      </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Leveraging scalability, durability and connectivity, C-Power ACBs integrate technological aspects to enhance uptime and energy efficiency.; Engineered for extreme tropical conditions, these ACBs excel in challenging environments, setting a market benchmark for performance and safety.; With a common door cut-out for the entire range and uniform height and depth for ACBs up to 4000A, they offer flexibility and ease of use.; Entire range offers High Short time withstand capacity, Icu=Ics=Icw for 1 sec to achieve total selectivity and full uptime of system.</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/C-Power_ACB_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>lk_ea_products/brochures/DU_DY_MCCB_Catalogue.pdf</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>The design is compact, optimising space and simplifying installation processes.; No load line bias ensures balanced power distribution, enhancing system efficiency.; Finger-proof terminals increase safety by preventing accidental contact, crucial in maintaining secure operations.; Phase barriers included with MCCBs enhance safety by effectively preventing electrical arcing between phases.</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/power-distribution-products/moulded-case-circuit-breaker-mccb/dz</t>
+          <t>https://www.lk-ea.com/products/power-distribution-products-lv-switchgear/switch-disconnectors-switch-disconnector-fuses-sdf/fn</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1466,45 +1454,45 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>DZ</t>
+          <t>FN</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Moulded Case Circuit Breaker Mccb</t>
+          <t>Switch Disconnectors Switch Disconnector Fuses Sdf</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>The dsine range stands out with its state-of-the-art design, user-friendly features, and a broad spectrum of protection mechanisms, marking it as a leader in the new generation of MCCBs (Moulded Case Circuit Breakers). Recognised for its ergonomic design, aesthetic appeal, and compactness, it is specifically engineered to perform reliably under extreme tropical conditions, offering consistent functionality in high ambient and humid environments. This makes the dsine MCCBs ideal for demanding settings, always meeting the evolving needs of our customers, a testament to our in-depth analysis and responsiveness to customer feedback.</t>
+          <t>Guaranteed performance in challenging environment coupled with unmatched reliability, these switching solutions are thriving in ruling in innumerable industrial and commercial installations. These switches are easy to install, use and inspect. All the switches also come with standard protective features such as terminal shrouds, phase barriers and high ground clearances.</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>The DZ range of Moulded Case Circuit Breakers (MCCB) is specifically designed to accommodate the complexities of modern electrical systems in contemporary installations. This range stands out due to its substantially higher fault-breaking capacities, addressing the rigorous demands of evolving power distribution requirements efficiently and effectively. Responding to the shifting expectations of customers who seek economical yet reliable solutions, we have developed the DZ range of MCCBs that can operate up to 800V AC, with exceptional fault-breaking capacities reaching up to 200kA at 415V AC. Available in both thermal magnetic and electronic versions, these MCCBs provide comprehensive protection, encompassing advanced current, voltage, frequency, power, and harmonic-based safeguards. This versatility empowers system designers and users to select and implement protection schemes that best fit their specific requirements, ensuring tailored and robust electrical safety.</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr"/>
+          <t>Guaranteed performance in challenging environment coupled with unmatched reliability, these switching solutions are thriving in ruling in innumerable industrial and commercial installations. These switches are easy to install, use and inspect. All the switches also come with standard protective. features such as terminal shrouds, phase barriers and high ground clearances.</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>images/FN.jpg</t>
+        </is>
+      </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>No load line bias ensures balanced power distribution, enhancing system efficiency.; Finger-proof terminals increase safety by preventing accidental contact, crucial for maintaining secure operations.; Phase barriers included with MCCBs enhance safety by effectively preventing electrical arcing between phases.; A wide range of common internal and external accessories is available, offering extensive customisation options to meet specific system requirements.</t>
+          <t>lk_ea_products/brochures/SD_&amp;_SDF_catalogue.pdf</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>images/DZ.jpg</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/DZ_MCCB_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>Door interlocking in ON position with defeat feature; Ample Space for termination in spacious SS enclosure version, no separate cable gland boxes required Clear ON/OFF indications.; Telescopic Shaft: Step-less depth adjustment; Suitable for aluminum termination.</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/power-distribution-products/moulded-case-circuit-breaker-mccb/dn</t>
+          <t>https://www.lk-ea.com/products/power-distribution-products-lv-switchgear/busbar-trunking-bbt/s-line</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1534,49 +1522,45 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>DN</t>
+          <t>S-Line</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Moulded Case Circuit Breaker Mccb</t>
+          <t>Busbar Trunking Bbt</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>The dsine range stands out with its state-of-the-art design, user-friendly features, and a broad spectrum of protection mechanisms, marking it as a leader in the new generation of MCCBs (Moulded Case Circuit Breakers). Recognised for its ergonomic design, aesthetic appeal, and compactness, it is specifically engineered to perform reliably under extreme tropical conditions, offering consistent functionality in high ambient and humid environments. This makes the dsine MCCBs ideal for demanding settings, always meeting the evolving needs of our customers, a testament to our in-depth analysis and responsiveness to customer feedback.</t>
+          <t>Lauritz Knudsen Electrical &amp; Automation is the leading supplier of the S-Line Busbar Trunking System in over 30 countries. Whether you're setting up a Metro line or an industrial complex, our S-Line Busbar Trunking products meet all your power distribution needs using copper or aluminium busbars. The S-Line offers bus duct systems from 250A to 6300A, featuring flexible designs with uniform Class-F insulation, excellent insulation, and higher joint overlapping for longer life, higher savings, and enhanced safety.</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>The dsine range stands out with its state-of-the-art design, user-friendly features, and a broad spectrum of protection mechanisms, marking it as a leader in the new generation of MCCBs (Moulded Case Circuit Breakers). Recognised for its ergonomic design, aesthetic appeal, and compactness, it is specifically engineered to perform reliably under extreme tropical conditions, offering consistent functionality in high ambient and humid environments. This makes the dsine MCCBs ideal for demanding settings, always meeting the evolving needs of our customers, a testament to our in-depth analysis and responsiveness to customer feedback. Understanding and anticipating the requirements of our customers, our contemporary range of MCCBs ensures complete customer satisfaction without compromise. Enhanced by a comprehensive selection of accessories, the dsine range provides complete solutions tailored to various customer applications. This integration ensures not only operational safety and reliability but also adds versatility to its use across different industries and systems, making it a robust choice for comprehensive electrical protection.</t>
+          <t>Lauritz Knudsen Electrical &amp; Automation is the leading supplier of the S-Line Busbar Trunking System in over 30 countries. Whether you're setting up a Metro line or an industrial complex, our S-Line Busbar Trunking products meet all your power distribution needs using copper or aluminium busbars. The S-Line offers bus duct systems from 250A to 6300A, featuring flexible designs with uniform Class-F insulation, excellent insulation, and higher joint overlapping for longer life, higher savings, and enhanced safety.</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Breaking Capacity: Options available at 25kA, 36kA, 50kA, 70kA, and 100kA, ensuring robust protection against high fault levels.; Variants: Choose from 3-pole or 4-pole versions to suit different circuit configurations.; Compliance: Fully compliant with IEC60947-2, EN60947-2, and IS/IEC60947-2 standards, ensuring international quality and safety benchmarks.; Protection Releases: Features both thermal-magnetic and microprocessor-based protection releases, offering precise and reliable circuit protection.</t>
+          <t>images/S-Line.jpg</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>No load line bias ensures balanced power distribution without preferential pathways.; Finger-proof terminals enhance safety by preventing accidental contact.; Suitable for DC applications, offering versatility across different electrical setups.; Phase barriers are provided with MCCBs to enhance safety by preventing electrical arcing between phases.; A wide range of common internal and external accessories is available, enabling easy integration and customisation to meet specific system requirements.</t>
+          <t>lk_ea_products/brochures/S-Line_BBT_catalogue.pdf</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>images/DN.jpg</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/dSine_MCCB_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>Joint block with maintenance-free twin-headed shear-off nut, ensuring secure connections without the need for ongoing maintenance.; Plug-in box with mechanical interlock and enhanced safety features, providing secure and easy installation with added protection.; A robust, safe, and reliable solution, designed to meet high standards of durability and performance in demanding environments.</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/power-distribution-products/moulded-case-circuit-breaker-mccb/dy</t>
+          <t>https://www.lk-ea.com/products/power-distribution-products-lv-switchgear/changeover-switch/c-line</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1606,45 +1590,45 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>DY</t>
+          <t>C-Line</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Moulded Case Circuit Breaker Mccb</t>
+          <t>Changeover Switch</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>The dsine range stands out with its state-of-the-art design, user-friendly features, and a broad spectrum of protection mechanisms, marking it as a leader in the new generation of MCCBs (Moulded Case Circuit Breakers). Recognised for its ergonomic design, aesthetic appeal, and compactness, it is specifically engineered to perform reliably under extreme tropical conditions, offering consistent functionality in high ambient and humid environments. This makes the dsine MCCBs ideal for demanding settings, always meeting the evolving needs of our customers, a testament to our in-depth analysis and responsiveness to customer feedback.</t>
+          <t>Electrical &amp; Automation (E&amp;A) offers you a unique series of Changeover Switches combining compactness with high performance &amp; customer convenience, thus, making it a state-of-the-art product in changeover technology</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>The DY Series represents the next generation of MCCBs, distinguished by its state-of-the-art design that combines contemporary, user-friendly features with outstanding ergonomics, aesthetics, and compactness. This series excels in functionality and form, making it an ideal choice for modern electrical infrastructure needs. In terms of compliance, the DY Series adheres to the latest international standards including IS/IEC 60947-2, IEC 60947-2, and EN 60947-2. Each product in the range carries the CE marking, affirming its quality and safety for use even in humid environments. Furthermore, equipped with a wide array of accessories, the series ensures operational safety, reliability, and versatility, meeting even the most demanding system requirements.</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr"/>
+          <t>C-LINE ensures a high standard of safety through its dependable switching mechanism, which operates independently of the user’s speed of operation. This mechanism incorporates a fail-safe mechanical interlock for all 3 positions in the I-0-II versions. Additionally, the inclusion of I-0-II position indicators directly on the handle and mechanism further enhances operational safet</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>images/C-Line.jpg</t>
+        </is>
+      </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>The design is compact, optimising space and simplifying installation processes.; No load line bias ensures balanced power distribution, enhancing system efficiency.; Finger-proof terminals increase safety by preventing accidental contact, crucial in maintaining secure operations.; Phase barriers included with MCCBs enhance safety by effectively preventing electrical arcing between phases.</t>
+          <t>lk_ea_products/brochures/C-Line_Online_Change_Over_Catalogue.pdf</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>images/DY.jpg</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/DU_DY_MCCB_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>Range from 40A to 2000A; Available in Open Execution, In SS Enclosure, Fused and Motorized version; User friendly features like; Staggered Terminals for ease in termination; Flippable handle for ease in operation; Dual Shaft position of centre and side; Fused version in form of kit; Higher Electrical and Mechanical Endurance; Higer Withstand Capacity; Frame 1 is DB mountable</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/power-distribution-products/moulded-case-circuit-breaker-mccb/du</t>
+          <t>https://www.lk-ea.com/products/motor-management-control/contactors/mcx</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1674,45 +1658,45 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>DU</t>
+          <t>MCX</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Moulded Case Circuit Breaker Mccb</t>
+          <t>Contactors</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>The dsine range stands out with its state-of-the-art design, user-friendly features, and a broad spectrum of protection mechanisms, marking it as a leader in the new generation of MCCBs (Moulded Case Circuit Breakers). Recognised for its ergonomic design, aesthetic appeal, and compactness, it is specifically engineered to perform reliably under extreme tropical conditions, offering consistent functionality in high ambient and humid environments. This makes the dsine MCCBs ideal for demanding settings, always meeting the evolving needs of our customers, a testament to our in-depth analysis and responsiveness to customer feedback.</t>
+          <t>Lauritz Knudsen Electrical and Automation’s extensive array of contactors offers unparalleled versatility to cater to a broad spectrum of demands across various applications. Designed for motor control, capacitor switching, supply changeover, and other single-phase or three-phase applications, our contactors provide the optimal solution tailored to your specific needs. This selection is further enhanced by our comprehensive line of thermal overload relays, ensuring robust protection and seamless integration with your systems. In addition to our core offerings, we provide a diverse range of accessories to enhance and complete your electrical setups. These include thermal overload relays, surge suppressors, and mechanical interlock kits, each designed to augment the functionality and safety of our contactor solutions. These accessories are engineered to the highest standards, offering both reliability and performance to support complex electrical infrastructures.</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>The DU Series represents the next generation of MCCBs, distinguished by its state-of-the-art design that combines contemporary, user-friendly features with outstanding ergonomics, aesthetics, and compactness. This series excels in functionality and form, making it an ideal choice for modern electrical infrastructure needs. In terms of compliance, the DU Series adheres to the latest international standards including IS/IEC 60947-2, IEC 60947-2, and EN 60947-2. Each product in the range carries the CE marking, affirming its quality and safety for use even in humid environments. Furthermore, equipped with a wide array of accessories, the series ensures operational safety, reliability, and versatility, meeting even the most demanding system requirements.</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr"/>
+          <t>The MCX range of 4-pole contactors, available from 18A to 900A AC-1, is extensively used with auto source transfer controllers to switch power from the main supply to backup sources such as DG (Diesel Generator) and UPS (Uninterruptible Power Supply).</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>images/MCX.jpg</t>
+        </is>
+      </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>The design is compact, optimising space and simplifying installation processes.; No load line bias ensures balanced power distribution, enhancing system efficiency.; Finger-proof terminals increase safety by preventing accidental contact, crucial in maintaining secure operations.; Phase barriers included with MCCBs enhance safety by effectively preventing electrical arcing between phases.</t>
+          <t>lk_ea_products/brochures/Motor_Management_&amp;_Control_Catalogue.pdf</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>images/DU.jpg</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/DU_DY_MCCB_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>The accessories are common across the range and compatible with the MNX range, simplifying inventory management and reducing the need to stock multiple types of accessories.; A detailed selection chart based on the diesel generator (DG) rating is provided, making it straightforward for users to select the appropriate contactor.; The compact mechanical interlock arrangement for models up to 80A enhances safety by preventing the simultaneous closure of both sets of contacts.</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/power-distribution-products/switch-disconnectors-switch-disconnector-fuses-sdf/fn</t>
+          <t>https://www.lk-ea.com/products/motor-management-control/contactors/mnx</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1742,45 +1726,45 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>MNX</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Switch Disconnectors Switch Disconnector Fuses Sdf</t>
+          <t>Contactors</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Guaranteed performance in challenging environment coupled with unmatched reliability, these switching solutions are thriving in ruling in innumerable industrial and commercial installations. These switches are easy to install, use and inspect. All the switches also come with standard protective features such as terminal shrouds, phase barriers and high ground clearances.</t>
+          <t>Lauritz Knudsen Electrical and Automation’s extensive array of contactors offers unparalleled versatility to cater to a broad spectrum of demands across various applications. Designed for motor control, capacitor switching, supply changeover, and other single-phase or three-phase applications, our contactors provide the optimal solution tailored to your specific needs. This selection is further enhanced by our comprehensive line of thermal overload relays, ensuring robust protection and seamless integration with your systems. In addition to our core offerings, we provide a diverse range of accessories to enhance and complete your electrical setups. These include thermal overload relays, surge suppressors, and mechanical interlock kits, each designed to augment the functionality and safety of our contactor solutions. These accessories are engineered to the highest standards, offering both reliability and performance to support complex electrical infrastructures.</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Guaranteed performance in challenging environment coupled with unmatched reliability, these switching solutions are thriving in ruling in innumerable industrial and commercial installations. These switches are easy to install, use and inspect. All the switches also come with standard protective. features such as terminal shrouds, phase barriers and high ground clearances.</t>
+          <t>MNX power contactors are primarily utilised in motor feeder and control system applications. With a range spanning from 9A to 650A (AC-3), they deliver dependable performance under various conditions, including high ambient temperatures and humidity. Additionally, accessories and spare parts are available for the entire range.</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>·Quad break contact system: Better arc quenching and higher electrical life of contacts</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr"/>
+          <t>images/MNX.jpg</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>lk_ea_products/brochures/Type_2_Co-Ordination_Catalogue.pdf</t>
+        </is>
+      </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>images/FN.jpg</t>
-        </is>
-      </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/SD_&amp;_SDF_catalogue.pdf</t>
-        </is>
-      </c>
+          <t>High reliability ensures consistent performance and minimal downtime in demanding applications.; Easy access terminals from 50A and above simplify installation and maintenance, enhancing operational efficiency.; Suitable for DC-1, DC-3, and DC-5 applications, offering versatile usage across various direct current systems.; Accessories and spares are available for the entire range, facilitating customization and long-term maintenance.</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/power-distribution-products/busbar-trunking-bbt/s-line</t>
+          <t>https://www.lk-ea.com/products/motor-management-control/contactors/mo</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1810,45 +1794,45 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>S-Line</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Busbar Trunking Bbt</t>
+          <t>Contactors</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Lauritz Knudsen Electrical &amp; Automation is the leading supplier of the S-Line Busbar Trunking System in over 30 countries. Whether you're setting up a Metro line or an industrial complex, our S-Line Busbar Trunking products meet all your power distribution needs using copper or aluminium busbars. The S-Line offers bus duct systems from 250A to 6300A, featuring flexible designs with uniform Class-F insulation, excellent insulation, and higher joint overlapping for longer life, higher savings, and enhanced safety.</t>
+          <t>Lauritz Knudsen Electrical and Automation’s extensive array of contactors offers unparalleled versatility to cater to a broad spectrum of demands across various applications. Designed for motor control, capacitor switching, supply changeover, and other single-phase or three-phase applications, our contactors provide the optimal solution tailored to your specific needs. This selection is further enhanced by our comprehensive line of thermal overload relays, ensuring robust protection and seamless integration with your systems. In addition to our core offerings, we provide a diverse range of accessories to enhance and complete your electrical setups. These include thermal overload relays, surge suppressors, and mechanical interlock kits, each designed to augment the functionality and safety of our contactor solutions. These accessories are engineered to the highest standards, offering both reliability and performance to support complex electrical infrastructures.</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Lauritz Knudsen Electrical &amp; Automation is the leading supplier of the S-Line Busbar Trunking System in over 30 countries. Whether you're setting up a Metro line or an industrial complex, our S-Line Busbar Trunking products meet all your power distribution needs using copper or aluminium busbars. The S-Line offers bus duct systems from 250A to 6300A, featuring flexible designs with uniform Class-F insulation, excellent insulation, and higher joint overlapping for longer life, higher savings, and enhanced safety.</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr"/>
+          <t>MO Contactors combine distinctive styling and visual appeal with dependable performance. Available in a range from 9A to 300A AC-3/3e, they are ideal for both general and specialised machinery. Their compact design saves panel space, and as RoHS compliant devices, they offer the advantages of being environmentally friendly and sustainable.</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>images/MO.jpg</t>
+        </is>
+      </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Joint block with maintenance-free twin-headed shear-off nut, ensuring secure connections without the need for ongoing maintenance.; Plug-in box with mechanical interlock and enhanced safety features, providing secure and easy installation with added protection.; A robust, safe, and reliable solution, designed to meet high standards of durability and performance in demanding environments.</t>
+          <t>lk_ea_products/brochures/Type_2_Co-Ordination_Catalogue.pdf</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>images/S-Line.jpg</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/S-Line_BBT_catalogue.pdf</t>
-        </is>
-      </c>
+          <t>Low panel footprint, saving valuable space in the control panel and allowing for more efficient use of available area.; Common spare parts for the MO family, minimising inventory requirements, reducing the need to stock multiple spare parts, simplifying maintenance, and lowering costs.; Type-2 chart available for motor applications, providing clear guidelines and ensuring reliable and optimised performance.; Lug and lugless termination options, offering flexibility in wiring methods and accommodating different installation preferences and requirements.; Shrouded design ensures user safety by protecting users from accidental contact with live components, enhancing operational safety.; Cassette type bridge facilitates easy inspection and maintenance, simplifying the process and reducing downtime, improving serviceability.</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/motor-management-control/industrial-starter/mn-starter</t>
+          <t>https://www.lk-ea.com/products/motor-management-control/contactors/mo0</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1878,45 +1862,45 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>MN Starter</t>
+          <t>MO0</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Industrial Starter</t>
+          <t>Contactors</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>MN range of industrial starters offers complete motor starting solution for industrial applications. These starters are time tested for reliable performance. They are a proven work horse for stand-alone motors in the industry.</t>
+          <t>Lauritz Knudsen Electrical and Automation’s extensive array of contactors offers unparalleled versatility to cater to a broad spectrum of demands across various applications. Designed for motor control, capacitor switching, supply changeover, and other single-phase or three-phase applications, our contactors provide the optimal solution tailored to your specific needs. This selection is further enhanced by our comprehensive line of thermal overload relays, ensuring robust protection and seamless integration with your systems. In addition to our core offerings, we provide a diverse range of accessories to enhance and complete your electrical setups. These include thermal overload relays, surge suppressors, and mechanical interlock kits, each designed to augment the functionality and safety of our contactor solutions. These accessories are engineered to the highest standards, offering both reliability and performance to support complex electrical infrastructures.</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>MN range of industrial starters offers complete motor starting solution for industrial applications. These starters are time tested for reliable performance. They are a proven work horse for stand-alone motors in the industry.</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr"/>
+          <t>MO0 control contactors are fundamental 4-pole contactors available with both AC and DC control. These contactors can be utilised for constructing control logic. With add-on blocks, these contactors can provide up to 8 auxiliary contacts. They are suitable for both industrial and commercial installations.</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>images/MO0.jpg</t>
+        </is>
+      </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Single Phasing Protection ensures the motor is safeguarded against damage caused by single phasing, preserving its longevity and preventing costly repairs.; Auto-Manual Reset Switch offers the convenience of automatic or manual reset options, allowing for flexibility in resetting the motor starter based on operational needs.; Trip Test Facility facilitates easy testing of the trip mechanism, enabling quick identification and resolution of potential issues to maintain optimal performance.; Electronic Timer in MN FASD for High Accuracy incorporates an electronic timer in the MN FASD model, delivering precise timing functionality for enhanced control and operational accuracy.</t>
+          <t>lk_ea_products/brochures/Motor_Management_&amp;_Control_Catalogue.pdf</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>images/MN Starter.jpg</t>
-        </is>
-      </c>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/Type_2_Co-Ordination_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>Finger-proof terminations ensure safe and secure auxiliary and control connections, reducing the risk of accidental contact.; Accessories are shared with the MO family of power contactors, thereby minimising inventory requirements and simplifying parts management.; Four auxiliary contacts are provided within a compact 45mm width, optimising space utilisation in installations.; An inbuilt surge suppressor in the MO0 DC model protects against voltage spikes, enhancing the reliability and lifespan of the contactor.; A common coil suitable for both 50Hz and 60Hz applications offers flexibility and reduces the need for multiple coil variants.</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/motor-management-control/motor-protection-circuit-breaker/mog</t>
+          <t>https://www.lk-ea.com/products/motor-management-control/contactors/mo-c</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1946,45 +1930,45 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>MOG</t>
+          <t>MO C</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Motor Protection Circuit Breaker</t>
+          <t>Contactors</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>The Supernova series motor protection circuit breaker (MPCB) from  Lauritz Knudsen Electrical and Automation seamlessly combines the functions of a moulded case circuit breaker (MCCB) and a thermal overload relay into a singular, highly compact unit. Featuring an adjustable current range dial with a precise maximum/minimum ratio of 1.4 to 1.6, the MPCB can be finely tuned to the rated current of the motor, ensuring optimal protection. This unit is specifically designed to safeguard against short circuits and overload conditions, enhancing the reliability and efficiency of motor operations. The design of the Supernova series MPCB incorporates overload relay functions within its compact framework, significantly reducing the required installation space and wiring complexity. This integration facilitates a more streamlined panel design, allowing for a reduction in overall panel size. Such design efficiency not only optimises space but also simplifies installation and maintenance processes, making it an ideal solution for diverse industrial applications.</t>
+          <t>Lauritz Knudsen Electrical and Automation’s extensive array of contactors offers unparalleled versatility to cater to a broad spectrum of demands across various applications. Designed for motor control, capacitor switching, supply changeover, and other single-phase or three-phase applications, our contactors provide the optimal solution tailored to your specific needs. This selection is further enhanced by our comprehensive line of thermal overload relays, ensuring robust protection and seamless integration with your systems. In addition to our core offerings, we provide a diverse range of accessories to enhance and complete your electrical setups. These include thermal overload relays, surge suppressors, and mechanical interlock kits, each designed to augment the functionality and safety of our contactor solutions. These accessories are engineered to the highest standards, offering both reliability and performance to support complex electrical infrastructures.</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>MOG MPCB combines short circuit protection and overload relay functionality in a highly compact unit. The MPCB is suitable for a wide range of small to medium motor loads that require high breaking capacity. Additionally, its compact size allows for a smaller installation area with reduced wiring space, thereby minimizing panel space.</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr"/>
+          <t>MO C Capacitor Duty Contactors are specially designed for capacitor switching applications. As capacitor switching is associated with high inrush current, the contactors are provided with damping resistors which limit the value of inrush current to a safe value. The contactors are used in APFC panels for switching power capacitors depending upon the amount of reactive power compensation required</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>images/MO C.jpg</t>
+        </is>
+      </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Compact design allows for a smaller installation area, saving valuable panel space.; Provides high breaking capacity for effective fault current interruption.; Ensures reliable short circuit protective coordination, reducing equipment damage.; Integrated features reduce wiring work, simplifying installation and cutting labour costs.; High switching durability ensures long-lasting performance in demanding applications.</t>
+          <t>lk_ea_products/brochures/Motor_Management_&amp;_Control_Catalogue.pdf</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>images/MOG.jpg</t>
-        </is>
-      </c>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/Type_2_Co-Ordination_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>Modular design saving precious panel space, optimising the utilisation of available area in electrical panels.; De-latching auxiliary contacts for improved switching, enhancing performance and reliability during operations.; Aesthetics and accessories same as MO Contactors, thus reducing the inventory by maintaining consistency across components.; Separate termination for damping resistors, ensuring easier installation and maintenance, and improving overall system organisation.</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/motor-management-control/electronic-motor-protection-relays/immr</t>
+          <t>https://www.lk-ea.com/products/motor-management-control/industrial-starter/mn-starter</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2014,45 +1998,45 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>IMMR</t>
+          <t>MN Starter</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Electronic Motor Protection Relays</t>
+          <t>Industrial Starter</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Motors play an important role in any industry and impact plant’s efficiency and energy consumption. It is, therefore, vital to protect your motor installations. Different motor installations require different types of protection. At Lauritz Knudsen Electrical &amp; Automation, we understand the need of the industry and offer an Intelligent Motor Management Relay (iMMR) for reliable protection, control and monitoring of electrical motors. Designed for use in the Intelligent motor control center, iMMR helps you to run your operation with reliable and effective protection against current/voltage variation, overload and earth fault. The iMMR provides detailed information about operational and diagnostic data in real-time that allows you to take corrective actions and avoid unexpected production downtime, losses and breakdowns. The compact design with built-in pre-programmed starter logic reduces manufacturing and commissioning time. iMMR suite software is available for easy and effective configuration, operation and diagnosis of the iMMR. Complex gate logic building is quite easy with the help of this iMMR suite software.</t>
+          <t>MN range of industrial starters offers complete motor starting solution for industrial applications. These starters are time tested for reliable performance. They are a proven work horse for stand-alone motors in the industry.</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Motors play an important role in any industry and impact plant’s efficiency and energy consumption. It is, therefore, vital to protect your motor installations. Different motor installations require different types of protection. At Lauritz Knudsen Electrical &amp; Automation, we understand the need of the industry and offer an Intelligent Motor Management Relay (iMMR) for reliable protection, control and monitoring of electrical motors.</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr"/>
+          <t>MN range of industrial starters offers complete motor starting solution for industrial applications. These starters are time tested for reliable performance. They are a proven work horse for stand-alone motors in the industry.</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>images/MN Starter.jpg</t>
+        </is>
+      </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Designed for use in the Intelligent motor control center, iMMR helps you to run your operation with reliable and effective protection against current/voltage variation, overload and earth fault.; The iMMR provides detailed information about operational and diagnostic data in real-time that allows you to take corrective actions and avoid unexpected production downtime, losses and breakdowns.; The compact design with built-in pre-programmed starter logic reduces manufacturing and commissioning time.; iMMR suite software is available for easy and effective configuration, operation and diagnosis of the iMMR.</t>
+          <t>lk_ea_products/brochures/Type_2_Co-Ordination_Catalogue.pdf</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>images/IMMR.jpg</t>
-        </is>
-      </c>
-      <c r="N24" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/iMMR_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>Single Phasing Protection ensures the motor is safeguarded against damage caused by single phasing, preserving its longevity and preventing costly repairs.; Auto-Manual Reset Switch offers the convenience of automatic or manual reset options, allowing for flexibility in resetting the motor starter based on operational needs.; Trip Test Facility facilitates easy testing of the trip mechanism, enabling quick identification and resolution of potential issues to maintain optimal performance.; Electronic Timer in MN FASD for High Accuracy incorporates an electronic timer in the MN FASD model, delivering precise timing functionality for enhanced control and operational accuracy.</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/industrial-automation-control/ac-drive/xd1000</t>
+          <t>https://www.lk-ea.com/products/motor-management-control/motor-protection-circuit-breaker/mog</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2082,45 +2066,45 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>xD1000</t>
+          <t>MOG</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Ac Drive</t>
+          <t>Motor Protection Circuit Breaker</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>With over four decades of engineering excellence, Lauritz Knudsen presents the xD Series AC Drives. This product, part of our Industrial Automation portfolio, goes beyond technology. It is engineered to deliver efficiency, reliability, and control. Whether you're managing HVAC systems, water treatment facilities, manufacturing lines, or process automation setups, the xD Series is designed to optimize motor control and enhance energy efficiency across a wide range of industrial applications.</t>
+          <t>The Supernova series motor protection circuit breaker (MPCB) from  Lauritz Knudsen Electrical and Automation seamlessly combines the functions of a moulded case circuit breaker (MCCB) and a thermal overload relay into a singular, highly compact unit. Featuring an adjustable current range dial with a precise maximum/minimum ratio of 1.4 to 1.6, the MPCB can be finely tuned to the rated current of the motor, ensuring optimal protection. This unit is specifically designed to safeguard against short circuits and overload conditions, enhancing the reliability and efficiency of motor operations. The design of the Supernova series MPCB incorporates overload relay functions within its compact framework, significantly reducing the required installation space and wiring complexity. This integration facilitates a more streamlined panel design, allowing for a reduction in overall panel size. Such design efficiency not only optimises space but also simplifies installation and maintenance processes, making it an ideal solution for diverse industrial applications.</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>The xD1000 Drive is a compact yet robust variable frequency drive (VFD) designed to meet the needs of various general-purpose applications such as pump, fan, conveyor &amp; compressors cutting across Industry &amp; Building segments. It is also capable to handle machine applications like F&amp;B machines, packaging machines, woodworking machines, textile machines, special purpose machines etc. It offers a user-friendly interface that simplifies installation and operation, making it accessible for both experienced and novice users. The xD1000 is equipped with advanced motor control features that enhance performance while optimizing energy consumption, contributing to lower operational costs. With its robust design and adaptability, the xD1000 Drive is an excellent choice for improving energy efficiency and reliability in diverse environments.</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr"/>
+          <t>MOG MPCB combines short circuit protection and overload relay functionality in a highly compact unit. The MPCB is suitable for a wide range of small to medium motor loads that require high breaking capacity. Additionally, its compact size allows for a smaller installation area with reduced wiring space, thereby minimizing panel space.</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>images/MOG.jpg</t>
+        </is>
+      </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Built in PID with 4 preset PID references, Wake up &amp; sleep mode, PID predictive speed; Auxiliary pump function (1 master + 1 slave); Torque boost; Stall prevention; Skip frequency; Catch on the fly (speed search / flying start); Fault inhibition (Fire mode); DC braking; Slip compensation; 8 preset speeds</t>
+          <t>lk_ea_products/brochures/Type_2_Co-Ordination_Catalogue.pdf</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>images/xD1000.jpg</t>
-        </is>
-      </c>
-      <c r="N25" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/xD_Series_Catalouge.pdf</t>
-        </is>
-      </c>
+          <t>Compact design allows for a smaller installation area, saving valuable panel space.; Provides high breaking capacity for effective fault current interruption.; Ensures reliable short circuit protective coordination, reducing equipment damage.; Integrated features reduce wiring work, simplifying installation and cutting labour costs.; High switching durability ensures long-lasting performance in demanding applications.</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/industrial-automation-control/ac-drive/xd2000</t>
+          <t>https://www.lk-ea.com/products/motor-management-control/electronic-motor-protection-relays/immr</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2150,45 +2134,45 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>xD2000</t>
+          <t>IMMR</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Ac Drive</t>
+          <t>Electronic Motor Protection Relays</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>With over four decades of engineering excellence, Lauritz Knudsen presents the xD Series AC Drives. This product, part of our Industrial Automation portfolio, goes beyond technology. It is engineered to deliver efficiency, reliability, and control. Whether you're managing HVAC systems, water treatment facilities, manufacturing lines, or process automation setups, the xD Series is designed to optimize motor control and enhance energy efficiency across a wide range of industrial applications.</t>
+          <t>Motors play an important role in any industry and impact plant’s efficiency and energy consumption. It is, therefore, vital to protect your motor installations. Different motor installations require different types of protection. At Lauritz Knudsen Electrical &amp; Automation, we understand the need of the industry and offer an Intelligent Motor Management Relay (iMMR) for reliable protection, control and monitoring of electrical motors. Designed for use in the Intelligent motor control center, iMMR helps you to run your operation with reliable and effective protection against current/voltage variation, overload and earth fault. The iMMR provides detailed information about operational and diagnostic data in real-time that allows you to take corrective actions and avoid unexpected production downtime, losses and breakdowns. The compact design with built-in pre-programmed starter logic reduces manufacturing and commissioning time. iMMR suite software is available for easy and effective configuration, operation and diagnosis of the iMMR. Complex gate logic building is quite easy with the help of this iMMR suite software.</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>The xD2000 Drive is a high-performance variable frequency drive designed to deliver exceptional control and efficiency for a variety of utility applications with its advanced control capabilities. The xD2000 allows for seamless integration into automation systems, enhancing overall operational performance. Its robust design ensures reliability in demanding environments, while features like energy-saving modes help reduce operational costs. The user-friendly interface simplifies setup and adjustments, making the xD2000 an ideal choice for both new installations and upgrades</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr"/>
+          <t>Motors play an important role in any industry and impact plant’s efficiency and energy consumption. It is, therefore, vital to protect your motor installations. Different motor installations require different types of protection. At Lauritz Knudsen Electrical &amp; Automation, we understand the need of the industry and offer an Intelligent Motor Management Relay (iMMR) for reliable protection, control and monitoring of electrical motors.</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>images/IMMR.jpg</t>
+        </is>
+      </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Inbuilt DC Reactor; Inbuilt EMC filter; Busbar plating to avoid chemical gas corrosion; Robust galvanic isolation; Inbuilt detachable LCD Display; Control of Permanent Magnet Synchronous Motors; Built in PID with 4 preset PID references, Wake up &amp; sleep mode, PID predictive speed; Booster Pump Control; Stall prevention; Skip frequency</t>
+          <t>lk_ea_products/brochures/iMMR_Catalogue.pdf</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>images/xD2000.jpg</t>
-        </is>
-      </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/xD_Series_Catalouge.pdf</t>
-        </is>
-      </c>
+          <t>Designed for use in the Intelligent motor control center, iMMR helps you to run your operation with reliable and effective protection against current/voltage variation, overload and earth fault.; The iMMR provides detailed information about operational and diagnostic data in real-time that allows you to take corrective actions and avoid unexpected production downtime, losses and breakdowns.; The compact design with built-in pre-programmed starter logic reduces manufacturing and commissioning time.; iMMR suite software is available for easy and effective configuration, operation and diagnosis of the iMMR.</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/industrial-automation-control/ac-drive/xd3000</t>
+          <t>https://www.lk-ea.com/products/industrial-automation-control/ac-drive/xd1000</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2218,7 +2202,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>xD3000</t>
+          <t>xD1000</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -2233,30 +2217,30 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>The xD3000 Drive is a versatile and high-performance variable frequency drive designed for a wide range of OEM applications. With its compact design and robust features, the xD3000 offers seamless integration into various industrial environments. It supports advanced motor control algorithms and includes built-in connectivity options, allowing for easy integration with automation systems. While, xD3000 is engineered for energy efficiency, safety of machines, it also help businesses to reduce operational costs &amp; maintaining optimal performance. Its user-friendly interface ensures quick setup and ease of use, making it an excellent choice for both new installations and retrofits.</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr"/>
+          <t>The xD1000 Drive is a compact yet robust variable frequency drive (VFD) designed to meet the needs of various general-purpose applications such as pump, fan, conveyor &amp; compressors cutting across Industry &amp; Building segments. It is also capable to handle machine applications like F&amp;B machines, packaging machines, woodworking machines, textile machines, special purpose machines etc. It offers a user-friendly interface that simplifies installation and operation, making it accessible for both experienced and novice users. The xD1000 is equipped with advanced motor control features that enhance performance while optimizing energy consumption, contributing to lower operational costs. With its robust design and adaptability, the xD1000 Drive is an excellent choice for improving energy efficiency and reliability in diverse environments.</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>images/xD1000.jpg</t>
+        </is>
+      </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Control of Permanent Magnet Synchronous Motors; Motor surge limit function for Old, Poor quality, Rewound Motors; Delinearization for Analog Inputs; High frequency range up to 599Hz for high-speed motors; Reference Addition, Subtraction &amp; Multiplication; Hoisting - External Brake Control, Load (External Weight) Measurement, High-speed Hoisting, Rope Slack; Motor / Generator Torque Limit; Load sharing; Line Contactor Control; Output Contactor Control</t>
+          <t>lk_ea_products/brochures/xD_Series_Catalouge.pdf</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>images/xD3000.jpg</t>
-        </is>
-      </c>
-      <c r="N27" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/xD_Series_Catalouge.pdf</t>
-        </is>
-      </c>
+          <t>Built in PID with 4 preset PID references, Wake up &amp; sleep mode, PID predictive speed; Auxiliary pump function (1 master + 1 slave); Torque boost; Stall prevention; Skip frequency; Catch on the fly (speed search / flying start); Fault inhibition (Fire mode); DC braking; Slip compensation; 8 preset speeds</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/industrial-automation-control/ac-drive/xd4000</t>
+          <t>https://www.lk-ea.com/products/industrial-automation-control/ac-drive/xd2000</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2286,7 +2270,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>xD4000</t>
+          <t>xD2000</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -2301,30 +2285,30 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>The xD4000 Drive is a highly advanced variable frequency drive designed for demanding applications in industries such as manufacturing, water treatment, and process automation. Featuring a powerful control algorithm, the xD4000 provides precise motor control and exceptional performance, ensuring optimal operation across various load conditions. Its extensive connectivity options enable easy integration with existing automation systems, while built-in energy-saving features help reduce operational costs. The xD4000 also boasts a user-friendly interface for quick setup and intuitive operation, making it an excellent choice for enhancing efficiency and productivity in any industrial environment.</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr"/>
+          <t>The xD2000 Drive is a high-performance variable frequency drive designed to deliver exceptional control and efficiency for a variety of utility applications with its advanced control capabilities. The xD2000 allows for seamless integration into automation systems, enhancing overall operational performance. Its robust design ensures reliability in demanding environments, while features like energy-saving modes help reduce operational costs. The user-friendly interface simplifies setup and adjustments, making the xD2000 an ideal choice for both new installations and upgrades</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>images/xD2000.jpg</t>
+        </is>
+      </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Inbuilt EMC Filter C2 &amp; C3; Inbuilt DC Reactor entire range; Inbuilt braking transistor upto 160kW HD; Interactive &amp; easy to use Graphical LCD keypad with help menu, battery for RTC &amp; QR code for troubleshooting; Abundant multifunctional IOs for field interface; Sucker rod function; Backspin sequence for PCP; Load sharing (Speed &amp; Torque); Backlash compensation; Built in PID with 4 preset PID references, Wake up &amp; sleep mode, Sleep Boost, PID predictive speed</t>
+          <t>lk_ea_products/brochures/xD_Series_Catalouge.pdf</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>images/xD4000.jpg</t>
-        </is>
-      </c>
-      <c r="N28" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/xD_Series_Catalouge.pdf</t>
-        </is>
-      </c>
+          <t>Inbuilt DC Reactor; Inbuilt EMC filter; Busbar plating to avoid chemical gas corrosion; Robust galvanic isolation; Inbuilt detachable LCD Display; Control of Permanent Magnet Synchronous Motors; Built in PID with 4 preset PID references, Wake up &amp; sleep mode, PID predictive speed; Booster Pump Control; Stall prevention; Skip frequency</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/industrial-automation-control/ac-drive/sx2000</t>
+          <t>https://www.lk-ea.com/products/industrial-automation-control/ac-drive/xd3000</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2354,7 +2338,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Sx2000</t>
+          <t>xD3000</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -2369,30 +2353,30 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>The Sx2000 drives offer a reliable solution for various industrial applications. With advanced control features and robust design, these drives provide efficient and precise motor control. They are engineered to deliver consistent performance in diverse operating conditions, making them a trusted choice for high-quality motor control solutions. Further enhancing their appeal, the Sx2000 drives are designed for easy integration into existing systems, offering scalable options to meet the specific needs of any application. They support a wide range of motor types, including AC induction motors, ensuring flexibility in deployment. This adaptability, combined with their user-friendly interface, simplifies setup and maintenance, helping to reduce downtime and operational costs.</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr"/>
+          <t>The xD3000 Drive is a versatile and high-performance variable frequency drive designed for a wide range of OEM applications. With its compact design and robust features, the xD3000 offers seamless integration into various industrial environments. It supports advanced motor control algorithms and includes built-in connectivity options, allowing for easy integration with automation systems. While, xD3000 is engineered for energy efficiency, safety of machines, it also help businesses to reduce operational costs &amp; maintaining optimal performance. Its user-friendly interface ensures quick setup and ease of use, making it an excellent choice for both new installations and retrofits.</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>images/xD3000.jpg</t>
+        </is>
+      </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>The integrated EMC filter minimizes electromagnetic interference, ensuring smoother operation.; The built-in DC reactor enhances energy efficiency and reduces harmonic distortion.; Output voltage control allows for precise adjustments to meet specific application requirements.; The KEB and Flying Start feature facilitates smooth restarts under dynamic loads without the need to reset.; Programmable user sequences enable customisable control for specific sequences and operations.; The multi-keypad interface offers user-friendly access for adjustments and monitoring.</t>
+          <t>lk_ea_products/brochures/xD_Series_Catalouge.pdf</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>images/Sx2000.jpg</t>
-        </is>
-      </c>
-      <c r="N29" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/AC_Drive_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>Control of Permanent Magnet Synchronous Motors; Motor surge limit function for Old, Poor quality, Rewound Motors; Delinearization for Analog Inputs; High frequency range up to 599Hz for high-speed motors; Reference Addition, Subtraction &amp; Multiplication; Hoisting - External Brake Control, Load (External Weight) Measurement, High-speed Hoisting, Rope Slack; Motor / Generator Torque Limit; Load sharing; Line Contactor Control; Output Contactor Control</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/industrial-automation-control/ac-drive/fx2000</t>
+          <t>https://www.lk-ea.com/products/industrial-automation-control/ac-drive/xd4000</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2422,7 +2406,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Fx2000</t>
+          <t>xD4000</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -2437,30 +2421,30 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>The Fx2000 drives are renowned for their robust construction and seamless functionality, establishing them as a top choice for industrial motor control applications. Engineered to deliver exceptional performance, these drives combine energy efficiency with reliable operation, meeting the varied demands of different industries. Their user-friendly features and advanced control capabilities make the Fx2000 drives an effective solution for boosting productivity and optimising processes. LK's Fx2000 drives are distinguished by their ability to provide efficient and customised motor control solutions, making them a reliable option for businesses aiming to enhance operational efficiency. With a focus on durability and adaptability, these drives support a range of industrial activities, ensuring that they not only meet but exceed the expectations of users in terms of performance and ease of use.</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr"/>
+          <t>The xD4000 Drive is a highly advanced variable frequency drive designed for demanding applications in industries such as manufacturing, water treatment, and process automation. Featuring a powerful control algorithm, the xD4000 provides precise motor control and exceptional performance, ensuring optimal operation across various load conditions. Its extensive connectivity options enable easy integration with existing automation systems, while built-in energy-saving features help reduce operational costs. The xD4000 also boasts a user-friendly interface for quick setup and intuitive operation, making it an excellent choice for enhancing efficiency and productivity in any industrial environment.</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>images/xD4000.jpg</t>
+        </is>
+      </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Brake control manages braking mechanisms efficiently, ensuring quick and safe stops that enhance operational safety and reduce wear on the system.; Kinetic energy buffering captures and reuses energy, which enhances overall efficiency during dynamic operations and reduces power consumption.; Output voltage control allows for precise voltage adjustments, optimising motor performance and ensuring optimal energy use.; The regeneration evasion function for press applications prevents energy backflow, improving both safety and equipment longevity in demanding industrial settings.</t>
+          <t>lk_ea_products/brochures/xD_Series_Catalouge.pdf</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>images/Fx2000.jpg</t>
-        </is>
-      </c>
-      <c r="N30" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/AC_Drive_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>Inbuilt EMC Filter C2 &amp; C3; Inbuilt DC Reactor entire range; Inbuilt braking transistor upto 160kW HD; Interactive &amp; easy to use Graphical LCD keypad with help menu, battery for RTC &amp; QR code for troubleshooting; Abundant multifunctional IOs for field interface; Sucker rod function; Backspin sequence for PCP; Load sharing (Speed &amp; Torque); Backlash compensation; Built in PID with 4 preset PID references, Wake up &amp; sleep mode, Sleep Boost, PID predictive speed</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/industrial-automation-control/ac-drive/hx2000</t>
+          <t>https://www.lk-ea.com/products/industrial-automation-control/ac-drive/sx2000</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2490,7 +2474,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Hx2000</t>
+          <t>Sx2000</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -2505,30 +2489,30 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Engineered to deliver exceptional precision and control, the Hx2000 AC drives enhance motor efficiency and productivity in a variety of HVAC applications. Featuring advanced technologies such as vector control and adaptive algorithms, these drives optimise motor performance, significantly reducing energy consumption. This makes them an ideal choice for industries aiming to streamline operations and cut costs, while maintaining high performance standards. The Hx2000 AC drives combine excellence and reliability, offering a robust solution suited to demanding industrial environments. They ensure smooth and consistent operation, day in and day out, providing businesses with the confidence that their motor-driven systems will perform reliably under various conditions. This reliability, coupled with enhanced efficiency, positions the Hx2000 drives as essential tools for improving operational effectiveness and sustainability.</t>
-        </is>
-      </c>
-      <c r="K31" t="inlineStr"/>
+          <t>The Sx2000 drives offer a reliable solution for various industrial applications. With advanced control features and robust design, these drives provide efficient and precise motor control. They are engineered to deliver consistent performance in diverse operating conditions, making them a trusted choice for high-quality motor control solutions. Further enhancing their appeal, the Sx2000 drives are designed for easy integration into existing systems, offering scalable options to meet the specific needs of any application. They support a wide range of motor types, including AC induction motors, ensuring flexibility in deployment. This adaptability, combined with their user-friendly interface, simplifies setup and maintenance, helping to reduce downtime and operational costs.</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>images/Sx2000.jpg</t>
+        </is>
+      </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Sub TitleThe pre-defined MACRO feature simplifies the initial setup process, enabling quick and efficient configuration tailored to specific applications, which accelerates deployment and reduces downtime.; Integrated EMC filtering enhances operational stability by reducing electromagnetic interference, ensuring compliance with international standards and protecting other sensitive electronics from disruptions.; Time Event Scheduling, alongside the Real Time Clock, automates operations based on precise timing, which optimises processes and improves overall system efficiency without manual intervention.; Multi Motor Control and the capability to operate a second motor from a single drive provide substantial cost savings and system simplification, allowing for streamlined management of multiple motor setups.</t>
+          <t>lk_ea_products/brochures/AC_Drive_Catalogue.pdf</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>images/Hx2000.jpg</t>
-        </is>
-      </c>
-      <c r="N31" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/AC_Drive_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>The integrated EMC filter minimizes electromagnetic interference, ensuring smoother operation.; The built-in DC reactor enhances energy efficiency and reduces harmonic distortion.; Output voltage control allows for precise adjustments to meet specific application requirements.; The KEB and Flying Start feature facilitates smooth restarts under dynamic loads without the need to reset.; Programmable user sequences enable customisable control for specific sequences and operations.; The multi-keypad interface offers user-friendly access for adjustments and monitoring.</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/industrial-automation-control/ac-drive/nx2000</t>
+          <t>https://www.lk-ea.com/products/industrial-automation-control/ac-drive/fx2000</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2558,7 +2542,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Nx2000</t>
+          <t>Fx2000</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -2573,30 +2557,30 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>SuThe Nx2000 AC drives represent a transformative advancement in industrial automation technology. Engineered to deliver unmatched performance and versatility, these drives are ideal for controlling electric motors across a wide range of industrial applications. With a focus on precision and reliability, the Nx2000 drives incorporate advanced features such as precise speed control, adaptive algorithms, and comprehensive protection mechanisms. These capabilities ensure optimal efficiency and enhanced safety during operation, making them a critical component in modern industrial setups. LK's longstanding expertise and commitment to quality are evident in the design and functionality of the Nx2000 AC drives. These drives empower industries to achieve new heights in productivity, efficiency, and operational excellence. Whether used in manufacturing, processing, or other demanding environments, the Nx2000 drives offer a robust solution that significantly improves system performance while maintaining high standards of energy efficiency and reliability.</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr"/>
+          <t>The Fx2000 drives are renowned for their robust construction and seamless functionality, establishing them as a top choice for industrial motor control applications. Engineered to deliver exceptional performance, these drives combine energy efficiency with reliable operation, meeting the varied demands of different industries. Their user-friendly features and advanced control capabilities make the Fx2000 drives an effective solution for boosting productivity and optimising processes. LK's Fx2000 drives are distinguished by their ability to provide efficient and customised motor control solutions, making them a reliable option for businesses aiming to enhance operational efficiency. With a focus on durability and adaptability, these drives support a range of industrial activities, ensuring that they not only meet but exceed the expectations of users in terms of performance and ease of use.</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>images/Fx2000.jpg</t>
+        </is>
+      </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>DIN rail mounting available up to 2.2kW provides a flexible and space-efficient installation option, simplifying setup in various industrial environments.; The integrated EMC filter reduces electromagnetic interference, ensuring stable and reliable operation of the drive under all conditions.; Side by side installation allows for compact use of space, enabling the placement of multiple drives close together without risk of overheating.; The remote expansion keypad enables convenient operation from a distance, improving accessibility and user comfort in managing drive settings and monitoring performance.</t>
+          <t>lk_ea_products/brochures/AC_Drive_Catalogue.pdf</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>images/Nx2000.jpg</t>
-        </is>
-      </c>
-      <c r="N32" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/AC_Drive_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>Brake control manages braking mechanisms efficiently, ensuring quick and safe stops that enhance operational safety and reduce wear on the system.; Kinetic energy buffering captures and reuses energy, which enhances overall efficiency during dynamic operations and reduces power consumption.; Output voltage control allows for precise voltage adjustments, optimising motor performance and ensuring optimal energy use.; The regeneration evasion function for press applications prevents energy backflow, improving both safety and equipment longevity in demanding industrial settings.</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/industrial-automation-control/soft-starters/xs1000</t>
+          <t>https://www.lk-ea.com/products/industrial-automation-control/ac-drive/hx2000</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2626,41 +2610,45 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>xS1000</t>
+          <t>Hx2000</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Soft Starters</t>
+          <t>Ac Drive</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>LK-EA provides a variety of soft starters engineered to manage the starting and stopping of induction motors. These soft starters minimise mechanical stress on both the motor and the connected equipment, ensuring smoother operation and prolonging the lifespan of the machinery. Additionally, they offer motor protection, advanced communication options, and energy-saving features. LK's soft starters are perfect for diverse industrial applications, delivering dependable and efficient motor control solutions.</t>
+          <t>With over four decades of engineering excellence, Lauritz Knudsen presents the xD Series AC Drives. This product, part of our Industrial Automation portfolio, goes beyond technology. It is engineered to deliver efficiency, reliability, and control. Whether you're managing HVAC systems, water treatment facilities, manufacturing lines, or process automation setups, the xD Series is designed to optimize motor control and enhance energy efficiency across a wide range of industrial applications.</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>The xS1000 Soft Starter is a solution for the controlled starting and stopping of induction motors. The xS1000 Soft Starter offers seamless integration, advanced motor protection features, and a user-friendly interface for easy operation. With its compact design and comprehensive functionality, the xS1000 Soft Starter is well-suited for diverse industrial applications, providing reliable and energy-efficient motor control. Its robust construction and advanced features make it a top choice for optimizing motor performance and enhancing operational efficiency.</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr"/>
-      <c r="L33" t="inlineStr"/>
+          <t>Engineered to deliver exceptional precision and control, the Hx2000 AC drives enhance motor efficiency and productivity in a variety of HVAC applications. Featuring advanced technologies such as vector control and adaptive algorithms, these drives optimise motor performance, significantly reducing energy consumption. This makes them an ideal choice for industries aiming to streamline operations and cut costs, while maintaining high performance standards. The Hx2000 AC drives combine excellence and reliability, offering a robust solution suited to demanding industrial environments. They ensure smooth and consistent operation, day in and day out, providing businesses with the confidence that their motor-driven systems will perform reliably under various conditions. This reliability, coupled with enhanced efficiency, positions the Hx2000 drives as essential tools for improving operational effectiveness and sustainability.</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>images/Hx2000.jpg</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>lk_ea_products/brochures/AC_Drive_Catalogue.pdf</t>
+        </is>
+      </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>images/xS1000.jpg</t>
-        </is>
-      </c>
-      <c r="N33" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/Soft_Starter_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>Sub TitleThe pre-defined MACRO feature simplifies the initial setup process, enabling quick and efficient configuration tailored to specific applications, which accelerates deployment and reduces downtime.; Integrated EMC filtering enhances operational stability by reducing electromagnetic interference, ensuring compliance with international standards and protecting other sensitive electronics from disruptions.; Time Event Scheduling, alongside the Real Time Clock, automates operations based on precise timing, which optimises processes and improves overall system efficiency without manual intervention.; Multi Motor Control and the capability to operate a second motor from a single drive provide substantial cost savings and system simplification, allowing for streamlined management of multiple motor setups.</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/industrial-automation-control/soft-starters/xs2000</t>
+          <t>https://www.lk-ea.com/products/industrial-automation-control/ac-drive/nx2000</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2690,41 +2678,45 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>xS2000</t>
+          <t>Nx2000</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Soft Starters</t>
+          <t>Ac Drive</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>LK-EA provides a variety of soft starters engineered to manage the starting and stopping of induction motors. These soft starters minimise mechanical stress on both the motor and the connected equipment, ensuring smoother operation and prolonging the lifespan of the machinery. Additionally, they offer motor protection, advanced communication options, and energy-saving features. LK's soft starters are perfect for diverse industrial applications, delivering dependable and efficient motor control solutions.</t>
+          <t>With over four decades of engineering excellence, Lauritz Knudsen presents the xD Series AC Drives. This product, part of our Industrial Automation portfolio, goes beyond technology. It is engineered to deliver efficiency, reliability, and control. Whether you're managing HVAC systems, water treatment facilities, manufacturing lines, or process automation setups, the xD Series is designed to optimize motor control and enhance energy efficiency across a wide range of industrial applications.</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>The xS2000 Soft Starter engineered to ensure smooth and efficient motor control while mitigating issues associated with direct-on-line starting, such as high inrush currents and mechanical stress. The xS2000 Soft Starter features advanced motor protection, integrated bypass, and a user-friendly interface, offering seamless integration and easy operation. Its compact design and comprehensive functionality make it suitable for a wide array of industrial applications, delivering reliable and energy-efficient motor control. With its robust construction and advanced features, the xS2000 Soft Starter stands as a top choice for optimizing motor performance and ensuring operational excellence.</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr"/>
-      <c r="L34" t="inlineStr"/>
+          <t>SuThe Nx2000 AC drives represent a transformative advancement in industrial automation technology. Engineered to deliver unmatched performance and versatility, these drives are ideal for controlling electric motors across a wide range of industrial applications. With a focus on precision and reliability, the Nx2000 drives incorporate advanced features such as precise speed control, adaptive algorithms, and comprehensive protection mechanisms. These capabilities ensure optimal efficiency and enhanced safety during operation, making them a critical component in modern industrial setups. LK's longstanding expertise and commitment to quality are evident in the design and functionality of the Nx2000 AC drives. These drives empower industries to achieve new heights in productivity, efficiency, and operational excellence. Whether used in manufacturing, processing, or other demanding environments, the Nx2000 drives offer a robust solution that significantly improves system performance while maintaining high standards of energy efficiency and reliability.</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>images/Nx2000.jpg</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>lk_ea_products/brochures/AC_Drive_Catalogue.pdf</t>
+        </is>
+      </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>images/xS2000.jpg</t>
-        </is>
-      </c>
-      <c r="N34" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/Soft_Starter_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>DIN rail mounting available up to 2.2kW provides a flexible and space-efficient installation option, simplifying setup in various industrial environments.; The integrated EMC filter reduces electromagnetic interference, ensuring stable and reliable operation of the drive under all conditions.; Side by side installation allows for compact use of space, enabling the placement of multiple drives close together without risk of overheating.; The remote expansion keypad enables convenient operation from a distance, improving accessibility and user comfort in managing drive settings and monitoring performance.</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/industrial-automation-control/soft-starters/xs3000</t>
+          <t>https://www.lk-ea.com/products/industrial-automation-control/soft-starters/xs1000</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -2754,7 +2746,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>xS3000</t>
+          <t>xS1000</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -2769,26 +2761,26 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>The LK-EA xS3000 Soft Starter is a cutting-edge solution designed to efficiently control the Starting &amp; Stopping of three-phase induction motors, providing seamless and reliable operation while minimizing mechanical stress and power distribution issues. With its advanced motor protection features and intelligent control algorithms, the xS3000 ensures smooth and controlled motor starting and stopping, contributing to enhanced system longevity and reduced maintenance costs. Equipped with a user-friendly interface and comprehensive monitoring capabilities, this soft starter is an ideal choice for applications across various industries, offering optimal performance and energy efficiency.</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr"/>
-      <c r="L35" t="inlineStr"/>
-      <c r="M35" t="inlineStr">
-        <is>
-          <t>images/xS3000.jpg</t>
-        </is>
-      </c>
-      <c r="N35" t="inlineStr">
+          <t>The xS1000 Soft Starter is a solution for the controlled starting and stopping of induction motors. The xS1000 Soft Starter offers seamless integration, advanced motor protection features, and a user-friendly interface for easy operation. With its compact design and comprehensive functionality, the xS1000 Soft Starter is well-suited for diverse industrial applications, providing reliable and energy-efficient motor control. Its robust construction and advanced features make it a top choice for optimizing motor performance and enhancing operational efficiency.</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>images/xS1000.jpg</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
         <is>
           <t>lk_ea_products/brochures/Soft_Starter_Catalogue.pdf</t>
         </is>
       </c>
+      <c r="M35" t="inlineStr"/>
+      <c r="N35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/industrial-automation-control/soft-starters/xs4000</t>
+          <t>https://www.lk-ea.com/products/industrial-automation-control/soft-starters/xs2000</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -2818,7 +2810,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>xS4000</t>
+          <t>xS2000</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -2833,26 +2825,26 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>The xS4000 Soft Starter is designed to provide seamless and efficient control for induction motors. It offers advanced features such as integrated bypass, built-in motor protection, and a user-friendly interface, making it suitable for a wide range of industrial applications. The xS4000 Soft Starter also incorporates advanced communication options, energy optimization capabilities, and robust construction, ensuring reliable and smooth motor operations while minimizing wear and tear. With its comprehensive set of features, the xS4000 Soft Starter stands as a top choice for optimizing motor performance and ensuring operational excellence.</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr"/>
-      <c r="L36" t="inlineStr"/>
-      <c r="M36" t="inlineStr">
-        <is>
-          <t>images/xS4000.jpg</t>
-        </is>
-      </c>
-      <c r="N36" t="inlineStr">
+          <t>The xS2000 Soft Starter engineered to ensure smooth and efficient motor control while mitigating issues associated with direct-on-line starting, such as high inrush currents and mechanical stress. The xS2000 Soft Starter features advanced motor protection, integrated bypass, and a user-friendly interface, offering seamless integration and easy operation. Its compact design and comprehensive functionality make it suitable for a wide array of industrial applications, delivering reliable and energy-efficient motor control. With its robust construction and advanced features, the xS2000 Soft Starter stands as a top choice for optimizing motor performance and ensuring operational excellence.</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>images/xS2000.jpg</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
         <is>
           <t>lk_ea_products/brochures/Soft_Starter_Catalogue.pdf</t>
         </is>
       </c>
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/energy-management-products/power-quality-and-power-factor-correction/ultra-heavy-capacitors</t>
+          <t>https://www.lk-ea.com/products/industrial-automation-control/soft-starters/xs3000</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -2867,7 +2859,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Not Found on Category Page</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -2882,41 +2874,41 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Ultra Heavy Capacitors</t>
+          <t>xS3000</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Power Quality And Power Factor Correction</t>
+          <t>Soft Starters</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>Laurtiz Knudsen Electrical &amp; Automation provides a comprehensive selection of Power Factor Capacitors tailored to lower overall power usage and enhance system efficiency. Our solution not only aids in maintaining the necessary power factor but also contributes to reducing electricity costs. Engineered with top-notch safety features like self-healing technology and overpressure disconnector fuse, our capacitors ensure utmost safety. We offer various Capacitor technologies including Metallised Poly Propylene (MPP) and Aluminum Poly Propylene (APP) films. MPP Capacitors come in Standard Duty, Heavy Duty, and Super Heavy-Duty ranges. On the other hand, APP Capacitors are available in box configuration across APP and Ultra Heavy-Duty Capacitors ranges, featuring internal fuse elements for added protection.</t>
+          <t>LK-EA provides a variety of soft starters engineered to manage the starting and stopping of induction motors. These soft starters minimise mechanical stress on both the motor and the connected equipment, ensuring smoother operation and prolonging the lifespan of the machinery. Additionally, they offer motor protection, advanced communication options, and energy-saving features. LK's soft starters are perfect for diverse industrial applications, delivering dependable and efficient motor control solutions.</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>The LTXL ultra-heavy duty box capacitors are advanced Aluminium Poly Propylene type capacitors. They can withstand heavy load fluctuations, high inrush current and harmonics. They can be used in applications such as welding, steel rolling, etc., with heavy load fluctuations, high harmonic distortion levels (non-linear load &gt;15%) and systems with high dv / dt.</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr"/>
+          <t>The LK-EA xS3000 Soft Starter is a cutting-edge solution designed to efficiently control the Starting &amp; Stopping of three-phase induction motors, providing seamless and reliable operation while minimizing mechanical stress and power distribution issues. With its advanced motor protection features and intelligent control algorithms, the xS3000 ensures smooth and controlled motor starting and stopping, contributing to enhanced system longevity and reduced maintenance costs. Equipped with a user-friendly interface and comprehensive monitoring capabilities, this soft starter is an ideal choice for applications across various industries, offering optimal performance and energy efficiency.</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>images/xS3000.jpg</t>
+        </is>
+      </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Suitable for harsh environments with heavy load fluctuations and high thermal loading like steel plants, automobile, cement plants, and fabrication industries.; Ideal for mid to large-scale heavy industrial applications.; Extended long life of 300,000 hours, reducing maintenance frequency and costs.; Designed to withstand Indian tropical conditions with temperatures up to 70°C, ensuring optimal performance in challenging environments.</t>
+          <t>lk_ea_products/brochures/Soft_Starter_Catalogue.pdf</t>
         </is>
       </c>
       <c r="M37" t="inlineStr"/>
-      <c r="N37" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/PQS_Catalogue_Domastic_01.pdf</t>
-        </is>
-      </c>
+      <c r="N37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/energy-management-products/power-quality-and-power-factor-correction/heavy-duty-capacitors</t>
+          <t>https://www.lk-ea.com/products/industrial-automation-control/soft-starters/xs4000</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2931,7 +2923,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Downloaded</t>
+          <t>Not Found on Category Page</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -2946,45 +2938,37 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Heavy Duty Capacitors</t>
+          <t>xS4000</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Power Quality And Power Factor Correction</t>
+          <t>Soft Starters</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>Laurtiz Knudsen Electrical &amp; Automation provides a comprehensive selection of Power Factor Capacitors tailored to lower overall power usage and enhance system efficiency. Our solution not only aids in maintaining the necessary power factor but also contributes to reducing electricity costs. Engineered with top-notch safety features like self-healing technology and overpressure disconnector fuse, our capacitors ensure utmost safety. We offer various Capacitor technologies including Metallised Poly Propylene (MPP) and Aluminum Poly Propylene (APP) films. MPP Capacitors come in Standard Duty, Heavy Duty, and Super Heavy-Duty ranges. On the other hand, APP Capacitors are available in box configuration across APP and Ultra Heavy-Duty Capacitors ranges, featuring internal fuse elements for added protection.</t>
+          <t>LK-EA provides a variety of soft starters engineered to manage the starting and stopping of induction motors. These soft starters minimise mechanical stress on both the motor and the connected equipment, ensuring smoother operation and prolonging the lifespan of the machinery. Additionally, they offer motor protection, advanced communication options, and energy-saving features. LK's soft starters are perfect for diverse industrial applications, delivering dependable and efficient motor control solutions.</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>E&amp;A’s Heavy-Duty Capacitors are metalized polypropylene capacitors available from 1-33.1 kVAr in cylindrical and from 1-50 kVAr in box type construction. These capacitors have an inrush current withstand of 300 In and an overload withstand capacity of 1.8 In. These capacitors have all the features of standard capacitors like over pressure disconnector and self-healing.</t>
+          <t>The xS4000 Soft Starter is designed to provide seamless and efficient control for induction motors. It offers advanced features such as integrated bypass, built-in motor protection, and a user-friendly interface, making it suitable for a wide range of industrial applications. The xS4000 Soft Starter also incorporates advanced communication options, energy optimization capabilities, and robust construction, ensuring reliable and smooth motor operations while minimizing wear and tear. With its comprehensive set of features, the xS4000 Soft Starter stands as a top choice for optimizing motor performance and ensuring operational excellence.</t>
         </is>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Available in 440 V, 480 V and 525 V.; Suitable for Industrial application; Designed for Indian conditions; Available in a wide range (1 kVAr to 33.1 kVAr in Cyl) &amp; (1 kVAr to 50 kVAr in Box) to meet demanding requirements.; Compact and space-saving design offers flexibility and easy assembly.; Operating Life 1,50,000 hrs</t>
-        </is>
-      </c>
-      <c r="M38" t="inlineStr">
-        <is>
-          <t>images/Heavy Duty Capacitors.jpg</t>
-        </is>
-      </c>
-      <c r="N38" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/PQS_Catalogue_Domastic_01.pdf</t>
-        </is>
-      </c>
+          <t>lk_ea_products/brochures/Soft_Starter_Catalogue.pdf</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr"/>
+      <c r="N38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/energy-management-products/power-quality-and-power-factor-correction/heavy-gas-filled-capacitors</t>
+          <t>https://www.lk-ea.com/products/energy-management-products/power-quality-and-power-factor-correction/ultra-heavy-capacitors</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3014,7 +2998,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Heavy - Gas filled Capacitors</t>
+          <t>Ultra Heavy Capacitors</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -3029,26 +3013,26 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Lauritz Knudsen Electrical &amp; Automation's Gas-filled Heavy Duty Plus capacitors come in cylindrical configurations, ranging from 3 to 30 kVAr. With a lifespan of 150,000 hours, these Heavy Duty Plus capacitors offer durability and reliability. After an extensive drying process, they are filled with an inert gas to safeguard against corrosion of internal components. These capacitors boast an impressive inrush withstand of 300 times In and an overload withstand capacity of 1.8 times In. Safety features include an over-pressure disconnector and self-healing mechanisms. Their compact design ensures efficient space utilization.</t>
+          <t>The LTXL ultra-heavy duty box capacitors are advanced Aluminium Poly Propylene type capacitors. They can withstand heavy load fluctuations, high inrush current and harmonics. They can be used in applications such as welding, steel rolling, etc., with heavy load fluctuations, high harmonic distortion levels (non-linear load &gt;15%) and systems with high dv / dt.</t>
         </is>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Available in 440V, 480V, and 525V variants, these capacitors offer flexibility with voltage options.; Suitable for heavy industrial applications, these capacitors provide reliable performance even in demanding environments.; Designed for Indian conditions ensure consistent performance and longevity.; Compact and space-saving design makes them suitable for installations where space is limited or where maximizing space utilization is important.</t>
-        </is>
-      </c>
-      <c r="M39" t="inlineStr"/>
-      <c r="N39" t="inlineStr">
-        <is>
           <t>lk_ea_products/brochures/PQS_Catalogue_Domastic_01.pdf</t>
         </is>
       </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>Suitable for harsh environments with heavy load fluctuations and high thermal loading like steel plants, automobile, cement plants, and fabrication industries.; Ideal for mid to large-scale heavy industrial applications.; Extended long life of 300,000 hours, reducing maintenance frequency and costs.; Designed to withstand Indian tropical conditions with temperatures up to 70°C, ensuring optimal performance in challenging environments.</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/energy-management-products/apfc-relays/etasmart</t>
+          <t>https://www.lk-ea.com/products/energy-management-products/power-quality-and-power-factor-correction/heavy-duty-capacitors</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3078,45 +3062,45 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>ETASMART</t>
+          <t>Heavy Duty Capacitors</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Apfc Relays</t>
+          <t>Power Quality And Power Factor Correction</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>The etaSMART APFC Controller rectifies power factor automatically through the connection and disconnection of capacitors. Equipped with a specially formulated optimisation program embedded in its microcontroller, it guarantees precise power factor regulation at the designated set point, ensuring smooth and uninterrupted operation.</t>
+          <t>Laurtiz Knudsen Electrical &amp; Automation provides a comprehensive selection of Power Factor Capacitors tailored to lower overall power usage and enhance system efficiency. Our solution not only aids in maintaining the necessary power factor but also contributes to reducing electricity costs. Engineered with top-notch safety features like self-healing technology and overpressure disconnector fuse, our capacitors ensure utmost safety. We offer various Capacitor technologies including Metallised Poly Propylene (MPP) and Aluminum Poly Propylene (APP) films. MPP Capacitors come in Standard Duty, Heavy Duty, and Super Heavy-Duty ranges. On the other hand, APP Capacitors are available in box configuration across APP and Ultra Heavy-Duty Capacitors ranges, featuring internal fuse elements for added protection.</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>The etaSMART APFC Controller rectifies power factor automatically through the connection and disconnection of capacitors. Equipped with a specially formulated optimization program embedded in its microcontroller, it guarantees precise power factor regulation at the designated set point, ensuring smooth and uninterrupted operation.</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr"/>
+          <t>E&amp;A’s Heavy-Duty Capacitors are metalized polypropylene capacitors available from 1-33.1 kVAr in cylindrical and from 1-50 kVAr in box type construction. These capacitors have an inrush current withstand of 300 In and an overload withstand capacity of 1.8 In. These capacitors have all the features of standard capacitors like over pressure disconnector and self-healing.</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>images/Heavy Duty Capacitors.jpg</t>
+        </is>
+      </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>It caters to a wide range of setups with both 2 and 4 quadrant operation capabilities, accommodating sites with or without solar plants.; Simplifies setup procedures, making it easy to program the controller automatically, saving time and effort.; With CT Secondary selection options, users can tailor current measurement to suit specific site requirements, enhancing accuracy and efficiency.; Automatic detection and correction of CT polarity in 2 quadrant mode ensure seamless operation and minimise the risk of errors, promoting consistent performance.</t>
+          <t>lk_ea_products/brochures/PQS_Catalogue_Domastic_01.pdf</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>images/ETASMART.jpg</t>
-        </is>
-      </c>
-      <c r="N40" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/APFC_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>Available in 440 V, 480 V and 525 V.; Suitable for Industrial application; Designed for Indian conditions; Available in a wide range (1 kVAr to 33.1 kVAr in Cyl) &amp; (1 kVAr to 50 kVAr in Box) to meet demanding requirements.; Compact and space-saving design offers flexibility and easy assembly.; Operating Life 1,50,000 hrs</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/mcb-rccb-distribution-boards/miniature-circuit-breaker-mcb/exora</t>
+          <t>https://www.lk-ea.com/products/energy-management-products/power-quality-and-power-factor-correction/heavy-gas-filled-capacitors</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3131,7 +3115,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Downloaded</t>
+          <t>Not Found on Category Page</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -3146,45 +3130,41 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Exora</t>
+          <t>Heavy - Gas filled Capacitors</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Miniature Circuit Breaker Mcb</t>
+          <t>Power Quality And Power Factor Correction</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>Protection and Control devices offered in this range provide safety at your home and at your workplace. It encompasses a suite of devices designed to safeguard your home against potential risks, ensuring peace of mind for you and your family.</t>
+          <t>Laurtiz Knudsen Electrical &amp; Automation provides a comprehensive selection of Power Factor Capacitors tailored to lower overall power usage and enhance system efficiency. Our solution not only aids in maintaining the necessary power factor but also contributes to reducing electricity costs. Engineered with top-notch safety features like self-healing technology and overpressure disconnector fuse, our capacitors ensure utmost safety. We offer various Capacitor technologies including Metallised Poly Propylene (MPP) and Aluminum Poly Propylene (APP) films. MPP Capacitors come in Standard Duty, Heavy Duty, and Super Heavy-Duty ranges. On the other hand, APP Capacitors are available in box configuration across APP and Ultra Heavy-Duty Capacitors ranges, featuring internal fuse elements for added protection.</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Protection and Control devices offered in this range provide safety at your home and at your workplace. Low Watt loss of these products reduces the amount of electricity consumed and results in low electricity expense. The new range of Modular Devices – EXORA –ensures a safe environment around you.</t>
+          <t>Lauritz Knudsen Electrical &amp; Automation's Gas-filled Heavy Duty Plus capacitors come in cylindrical configurations, ranging from 3 to 30 kVAr. With a lifespan of 150,000 hours, these Heavy Duty Plus capacitors offer durability and reliability. After an extensive drying process, they are filled with an inert gas to safeguard against corrosion of internal components. These capacitors boast an impressive inrush withstand of 300 times In and an overload withstand capacity of 1.8 times In. Safety features include an over-pressure disconnector and self-healing mechanisms. Their compact design ensures efficient space utilization.</t>
         </is>
       </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr">
         <is>
-          <t>MCB is the best option to use for the protection of wiring installations against short-circuits and over-load with lots of advantages over regular Fuse unit.; It is a protection device to safeguard both your Life and Valuable Property.</t>
+          <t>lk_ea_products/brochures/PQS_Catalogue_Domastic_01.pdf</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>images/Exora.jpg</t>
-        </is>
-      </c>
-      <c r="N41" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/Exora_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>Available in 440V, 480V, and 525V variants, these capacitors offer flexibility with voltage options.; Suitable for heavy industrial applications, these capacitors provide reliable performance even in demanding environments.; Designed for Indian conditions ensure consistent performance and longevity.; Compact and space-saving design makes them suitable for installations where space is limited or where maximizing space utilization is important.</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/mcb-rccb-distribution-boards/miniature-circuit-breaker-mcb/au</t>
+          <t>https://www.lk-ea.com/products/energy-management-products/apfc-relays/etasmart</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3214,45 +3194,45 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>ETASMART</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Miniature Circuit Breaker Mcb</t>
+          <t>Apfc Relays</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>Protection and Control devices offered in this range provide safety at your home and at your workplace. It encompasses a suite of devices designed to safeguard your home against potential risks, ensuring peace of mind for you and your family.</t>
+          <t>The etaSMART APFC Controller rectifies power factor automatically through the connection and disconnection of capacitors. Equipped with a specially formulated optimisation program embedded in its microcontroller, it guarantees precise power factor regulation at the designated set point, ensuring smooth and uninterrupted operation.</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>AU Solutions comprises protection, control, and monitoring devices crafted from accumulated knowledge. From safeguarding against overload and earth leakage to handling lightning and switching surges, this collection exceeds expectations, catering to both current and future needs.</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr"/>
+          <t>The etaSMART APFC Controller rectifies power factor automatically through the connection and disconnection of capacitors. Equipped with a specially formulated optimization program embedded in its microcontroller, it guarantees precise power factor regulation at the designated set point, ensuring smooth and uninterrupted operation.</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>images/ETASMART.jpg</t>
+        </is>
+      </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Providing protection against overload and short-circuit faults.; The AU range of MCBs is designed to offer the lowest watt loss in the industry. This conserves power and helps you save much more than money.</t>
+          <t>lk_ea_products/brochures/APFC_Catalogue.pdf</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>images/AU.jpg</t>
-        </is>
-      </c>
-      <c r="N42" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/AU-MCB,RCCB,RCBO_Catalouge.pdf</t>
-        </is>
-      </c>
+          <t>It caters to a wide range of setups with both 2 and 4 quadrant operation capabilities, accommodating sites with or without solar plants.; Simplifies setup procedures, making it easy to program the controller automatically, saving time and effort.; With CT Secondary selection options, users can tailor current measurement to suit specific site requirements, enhancing accuracy and efficiency.; Automatic detection and correction of CT polarity in 2 quadrant mode ensure seamless operation and minimise the risk of errors, promoting consistent performance.</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/mcb-rccb-distribution-boards/residual-current-operated-circuit-breaker-rcbo/au</t>
+          <t>https://www.lk-ea.com/products/mcb-rccb-distribution-boards/miniature-circuit-breaker-mcb/exora</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3282,41 +3262,45 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>Exora</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Residual Current Operated Circuit Breaker Rcbo</t>
+          <t>Miniature Circuit Breaker Mcb</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>As India's leading manufacturer of low-voltage and medium-voltage switchgear for industries, buildings, homes and agriculture segments; we offer more than expected – meeting your needs of today and tomorrow.</t>
+          <t>Protection and Control devices offered in this range provide safety at your home and at your workplace. It encompasses a suite of devices designed to safeguard your home against potential risks, ensuring peace of mind for you and your family.</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>As India's leading manufacturer of low-voltage and medium-voltage switchgear for industries, buildings, homes and agriculture segments; we offer more than expected – meeting your needs of today and tomorrow.</t>
-        </is>
-      </c>
-      <c r="K43" t="inlineStr"/>
-      <c r="L43" t="inlineStr"/>
+          <t>Protection and Control devices offered in this range provide safety at your home and at your workplace. Low Watt loss of these products reduces the amount of electricity consumed and results in low electricity expense. The new range of Modular Devices – EXORA –ensures a safe environment around you.</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>images/Exora.jpg</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>lk_ea_products/brochures/Exora_Catalogue.pdf</t>
+        </is>
+      </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>images/AU.jpg</t>
-        </is>
-      </c>
-      <c r="N43" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/AU-MCB,RCCB,RCBO_Catalouge.pdf</t>
-        </is>
-      </c>
+          <t>MCB is the best option to use for the protection of wiring installations against short-circuits and over-load with lots of advantages over regular Fuse unit.; It is a protection device to safeguard both your Life and Valuable Property.</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/mcb-rccb-distribution-boards/residual-current-circuit-breaker-rccb/exora</t>
+          <t>https://www.lk-ea.com/products/mcb-rccb-distribution-boards/miniature-circuit-breaker-mcb/au</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3346,45 +3330,45 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Exora</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Residual Current Circuit Breaker Rccb</t>
+          <t>Miniature Circuit Breaker Mcb</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>Protection and Control devices offered in this range provide safety at your home and at your workplace. Low Watt loss of these products reduces the amount of electricity consumed and results in low electricity expenses. Features such as Biconnected and Two Position DIN Clip provide flexibility and ease of operation. Spanning from shielding against overloads and earth leakage to countering lightning and switching surges, this assortment surpasses expectations, catering to both current and future requirements.</t>
+          <t>Protection and Control devices offered in this range provide safety at your home and at your workplace. It encompasses a suite of devices designed to safeguard your home against potential risks, ensuring peace of mind for you and your family.</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Protection and Control devices offered in this range provide safety at your home and at your workplace. Low Watt loss of these products reduces the amount of electricity consumed and results in low electricity expenses. Features such as Biconnected and Two Position DIN Clip provide flexibility and ease of operation.</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr"/>
+          <t>AU Solutions comprises protection, control, and monitoring devices crafted from accumulated knowledge. From safeguarding against overload and earth leakage to handling lightning and switching surges, this collection exceeds expectations, catering to both current and future needs.</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>images/AU.jpg</t>
+        </is>
+      </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Residual Current Circuit Breakers provide protection against earth leakage fault.; They ensure safety of human life in case of earth leakage fault and protection against electric shock.</t>
+          <t>lk_ea_products/brochures/AU-MCB,RCCB,RCBO_Catalouge.pdf</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>images/Exora.jpg</t>
-        </is>
-      </c>
-      <c r="N44" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/Exora_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>Providing protection against overload and short-circuit faults.; The AU range of MCBs is designed to offer the lowest watt loss in the industry. This conserves power and helps you save much more than money.</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/mcb-rccb-distribution-boards/1phase-3phase-automatic-changeover-with-current-limiter-accl/au</t>
+          <t>https://www.lk-ea.com/products/mcb-rccb-distribution-boards/residual-current-operated-circuit-breaker-rcbo/au</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3419,40 +3403,36 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>1Phase 3Phase Automatic Changeover With Current Limiter Accl</t>
+          <t>Residual Current Operated Circuit Breaker Rcbo</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>Protection and Control devices offered in this range provide safety at your home and at your workplace. It encompasses a suite of devices designed to safeguard your home against potential risks, ensuring peace of mind for you and your family.</t>
+          <t>As India's leading manufacturer of low-voltage and medium-voltage switchgear for industries, buildings, homes and agriculture segments; we offer more than expected – meeting your needs of today and tomorrow.</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Lauritz Knudsen Electrical and Automation stands as India's foremost producer of low and medium-voltage switchgear for industrial, commercial, residential, and agricultural applications. From the beginning, we have attentively listened to, observed, and understood our customers' requirements. This insight has led to the creation of AU Solutions, a comprehensive range of devices for protection, control, and monitoring. From protection against overload and earth leakage to lightning and switching surges, this range offers more than expected – meeting your needs of today and tomorrow.</t>
-        </is>
-      </c>
-      <c r="K45" t="inlineStr"/>
+          <t>As India's leading manufacturer of low-voltage and medium-voltage switchgear for industries, buildings, homes and agriculture segments; we offer more than expected – meeting your needs of today and tomorrow.</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>images/AU.jpg</t>
+        </is>
+      </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Ideal for efficient power distribution in high-rise apartments, townships, and commercial buildings.; Three pairs of terminals: two for connecting single-phase supplies (main and backup) and one for connecting the single-phase load.; Switches the load to backup/generator supply when the main/default supply fails.; Automatically reverts to the default supply upon its resumption for seamless power management.</t>
-        </is>
-      </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>images/AU.jpg</t>
-        </is>
-      </c>
-      <c r="N45" t="inlineStr">
-        <is>
           <t>lk_ea_products/brochures/AU-MCB,RCCB,RCBO_Catalouge.pdf</t>
         </is>
       </c>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/mcb-rccb-distribution-boards/modular-contactor/au</t>
+          <t>https://www.lk-ea.com/products/mcb-rccb-distribution-boards/residual-current-circuit-breaker-rccb/exora</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3482,41 +3462,45 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>Exora</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Modular Contactor</t>
+          <t>Residual Current Circuit Breaker Rccb</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>AU Solutions is a range of protection, control and monitoring devices born from the learning gained. From protection against overload and earth leakage to lightning and switching surges, this range offers more than expected – meeting your needs of today and tomorrow.</t>
+          <t>Protection and Control devices offered in this range provide safety at your home and at your workplace. Low Watt loss of these products reduces the amount of electricity consumed and results in low electricity expenses. Features such as Biconnected and Two Position DIN Clip provide flexibility and ease of operation. Spanning from shielding against overloads and earth leakage to countering lightning and switching surges, this assortment surpasses expectations, catering to both current and future requirements.</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>AU Solutions is a range of protection, control and monitoring devices born from the learning gained. From protection against overload and earth leakage to lightning and switching surges, this range offers more than expected – meeting your needs of today and tomorrow.</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr"/>
-      <c r="L46" t="inlineStr"/>
+          <t>Protection and Control devices offered in this range provide safety at your home and at your workplace. Low Watt loss of these products reduces the amount of electricity consumed and results in low electricity expenses. Features such as Biconnected and Two Position DIN Clip provide flexibility and ease of operation.</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>images/Exora.jpg</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>lk_ea_products/brochures/Exora_Catalogue.pdf</t>
+        </is>
+      </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>images/AU.jpg</t>
-        </is>
-      </c>
-      <c r="N46" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/AU-MCB,RCCB,RCBO_Catalouge.pdf</t>
-        </is>
-      </c>
+          <t>Residual Current Circuit Breakers provide protection against earth leakage fault.; They ensure safety of human life in case of earth leakage fault and protection against electric shock.</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/mcb-rccb-distribution-boards/surge-protective-devices-spd/au</t>
+          <t>https://www.lk-ea.com/products/mcb-rccb-distribution-boards/1phase-3phase-automatic-changeover-with-current-limiter-accl/au</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3551,40 +3535,40 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Surge Protective Devices Spd</t>
+          <t>1Phase 3Phase Automatic Changeover With Current Limiter Accl</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>AU Solutions is a range of protection, control and monitoring devices born from the learning gained. From protection against overload and earth leakage to lightning and switching surges, this range offers more than expected – meeting your needs of today and tomorrow.</t>
+          <t>Protection and Control devices offered in this range provide safety at your home and at your workplace. It encompasses a suite of devices designed to safeguard your home against potential risks, ensuring peace of mind for you and your family.</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>AU Solutions is a range of protection, control and monitoring devices born from the learning gained. From protection against overload and earth leakage to lightning and switching surges, this range offers more than expected – meeting your needs of today and tomorrow.</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr"/>
+          <t>Lauritz Knudsen Electrical and Automation stands as India's foremost producer of low and medium-voltage switchgear for industrial, commercial, residential, and agricultural applications. From the beginning, we have attentively listened to, observed, and understood our customers' requirements. This insight has led to the creation of AU Solutions, a comprehensive range of devices for protection, control, and monitoring. From protection against overload and earth leakage to lightning and switching surges, this range offers more than expected – meeting your needs of today and tomorrow.</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>images/AU.jpg</t>
+        </is>
+      </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>SPDs provide protection to electrical/electronic equipment against a brief overvoltage spike or disturbance on a power/signal waveform called a surge.; The AU Solutions range of SPDs provides protection against lightning and switching surges.</t>
+          <t>lk_ea_products/brochures/AU-MCB,RCCB,RCBO_Catalouge.pdf</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>images/AU.jpg</t>
-        </is>
-      </c>
-      <c r="N47" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/AU-MCB,RCCB,RCBO_Catalouge.pdf</t>
-        </is>
-      </c>
+          <t>Ideal for efficient power distribution in high-rise apartments, townships, and commercial buildings.; Three pairs of terminals: two for connecting single-phase supplies (main and backup) and one for connecting the single-phase load.; Switches the load to backup/generator supply when the main/default supply fails.; Automatically reverts to the default supply upon its resumption for seamless power management.</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/mcb-rccb-distribution-boards/isolators/exora</t>
+          <t>https://www.lk-ea.com/products/mcb-rccb-distribution-boards/modular-contactor/au</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -3614,45 +3598,41 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Exora</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Isolators</t>
+          <t>Modular Contactor</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>Lauritz Knudsen Electrical and Automation is India's leading manufacturer of low-voltage and medium-voltage switchgear for industries, buildings, homes and agriculture segments. Since the start of our journey, we have listened, observed and experienced our customers' needs. Salient features of this range – Quick Break Mechanism, True Contact Position Indicator, Energy Limitation Class 3 – enhance safety of human lives and precious belongings. Further, Low Watt loss of these products reduces the amount of electricity consumed and results in low electricity expense.</t>
+          <t>AU Solutions is a range of protection, control and monitoring devices born from the learning gained. From protection against overload and earth leakage to lightning and switching surges, this range offers more than expected – meeting your needs of today and tomorrow.</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Our new range of Modular Devices – EXORA – ensure a safe environment around you. Protection and Control devices offered in this range provide safety at your home and at your workplace. Salient features of this range – Quick Break Mechanism, True Contact Position Indicator, Energy Limitation Class 3 – enhance safety of human lives and precious belongings. Further, Low Watt loss of these products reduces the amount of electricity consumed and results in low electricity expense.</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr"/>
+          <t>AU Solutions is a range of protection, control and monitoring devices born from the learning gained. From protection against overload and earth leakage to lightning and switching surges, this range offers more than expected – meeting your needs of today and tomorrow.</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>images/AU.jpg</t>
+        </is>
+      </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>The isolator ensures that the circuit is entirely isolated, meaning no current can reach the load side when the isolator is turned OFF. This provides a high level of safety and prevents any unintended electrical flow, even if there is an impulse voltage.; Isolators are designed to make, carry, and break circuit current, allowing them to handle various electrical states. This versatility makes them essential for managing electrical installations and ensuring safe operation under different conditions.</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>images/Exora.jpg</t>
-        </is>
-      </c>
-      <c r="N48" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/Exora_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>lk_ea_products/brochures/AU-MCB,RCCB,RCBO_Catalouge.pdf</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/panel-accessories/time-switches/fmqt</t>
+          <t>https://www.lk-ea.com/products/mcb-rccb-distribution-boards/surge-protective-devices-spd/au</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -3667,7 +3647,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Not Found on Category Page</t>
+          <t>Downloaded</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -3682,41 +3662,45 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>FMQT</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Time Switches</t>
+          <t>Surge Protective Devices Spd</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>This advanced analogue &amp; digital time switches are designed to offer unparalleled convenience and reliability in managing electrical systems.</t>
+          <t>AU Solutions is a range of protection, control and monitoring devices born from the learning gained. From protection against overload and earth leakage to lightning and switching surges, this range offers more than expected – meeting your needs of today and tomorrow.</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>This advanced analogue time switch is designed to offer unparalleled convenience and reliability in managing electrical systems. With a robust power reserve lasting up to 150 hours, along with an inbuilt override facility, this switch ensures uninterrupted functionality even in unpredictable circumstances. Its tamper-proof sealing provision adds an extra layer of security, safeguarding against unauthorised access or meddling.</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr"/>
+          <t>AU Solutions is a range of protection, control and monitoring devices born from the learning gained. From protection against overload and earth leakage to lightning and switching surges, this range offers more than expected – meeting your needs of today and tomorrow.</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>images/AU.jpg</t>
+        </is>
+      </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Enjoy uninterrupted functionality during power outages or disruptions with a power reserve of up to 150 hours.; Easily adjust schedules or settings manually with the inbuilt override facility for added flexibility and convenience.; Ensure the integrity of your electrical systems with the tamper-proof sealing provision, safeguarding against unauthorised access or tampering.</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr"/>
-      <c r="N49" t="inlineStr">
-        <is>
-          <t>lk_ea_products/brochures/Panel_Accessories_Catalogue.pdf</t>
-        </is>
-      </c>
+          <t>lk_ea_products/brochures/AU-MCB,RCCB,RCBO_Catalouge.pdf</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>SPDs provide protection to electrical/electronic equipment against a brief overvoltage spike or disturbance on a power/signal waveform called a surge.; The AU Solutions range of SPDs provides protection against lightning and switching surges.</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>https://www.lk-ea.com/products/panel-accessories/push-buttons-indicating-lamps/gen-next-pro-22.5-mm</t>
+          <t>https://www.lk-ea.com/products/mcb-rccb-distribution-boards/isolators/exora</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -3746,40 +3730,640 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
+          <t>Exora</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Isolators</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Lauritz Knudsen Electrical and Automation is India's leading manufacturer of low-voltage and medium-voltage switchgear for industries, buildings, homes and agriculture segments. Since the start of our journey, we have listened, observed and experienced our customers' needs. Salient features of this range – Quick Break Mechanism, True Contact Position Indicator, Energy Limitation Class 3 – enhance safety of human lives and precious belongings. Further, Low Watt loss of these products reduces the amount of electricity consumed and results in low electricity expense.</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>Our new range of Modular Devices – EXORA – ensure a safe environment around you. Protection and Control devices offered in this range provide safety at your home and at your workplace. Salient features of this range – Quick Break Mechanism, True Contact Position Indicator, Energy Limitation Class 3 – enhance safety of human lives and precious belongings. Further, Low Watt loss of these products reduces the amount of electricity consumed and results in low electricity expense.</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>images/Exora.jpg</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>lk_ea_products/brochures/Exora_Catalogue.pdf</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>The isolator ensures that the circuit is entirely isolated, meaning no current can reach the load side when the isolator is turned OFF. This provides a high level of safety and prevents any unintended electrical flow, even if there is an impulse voltage.; Isolators are designed to make, carry, and break circuit current, allowing them to handle various electrical states. This versatility makes them essential for managing electrical installations and ensuring safe operation under different conditions.</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>https://www.lk-ea.com/products/pump-starters-and-controllers/starter/mk-starter</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Lauritz Knudsen</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Electrical Equipment</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Downloaded</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Downloaded</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>MK Starter</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Starter</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>Since 1960, Lauritz Knudsen Electrical &amp; Automation has been catering to the agriculture, domestic &amp; industrial sectors with a wide range of low motor protection solutions for pumps that help in reliable and efficient irrigation &amp; water management. Our wide range of Direct On-Line (DOL) Starter, Star-Delta Starters, Single Phase &amp; Three Phase variants are the ideal choice for agricultural pumping applications. Available for up to 35 HP pumps, the starters are designed to operate agriculture motors efficiently while offering reliable protection. The 3 phase Starters along with SPPR (single phasing protection relay) provide overload protection, protection from phase unbalance, single phasing, and phase reversal failures. The compact enclosure protects against dust, humidity and insects and is suitable for hot and humid environments. Easy to connect and operate, our Motor Starters are widely acceptable among farmers, industrial owners for individual pumping systems.</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>Lauritz Knudsen Electrical &amp; Automation began its legacy 70 years ago with the introduction of MK Starters, a cornerstone of reliability in motor control technology. To date, the brand has sold over 25 million units, a testament to the enduring trust and satisfaction of its customers. These starters have been designed to meet the demands of both Direct Online (DOL) and Star-Delta applications, ensuring versatility across a wide range of agricultural and industrial uses. The MK1 and MK2 series are distinguished by their wide-band coil operation, which enhances performance across varied voltage conditions. This feature, coupled with robust design and advanced protective mechanisms, makes MK Starters a preferred choice for ensuring optimal motor efficiency and longevity in demanding agricultural and industrial environments Available Range: MK1 Starters: Relay Range: Up to 13-22 A MK2 Starters: Relay Range: 20-32 A for higher current applications. Direct Online (DOL) Starters: Available up to 7.5hp. Star-Delta Starters: Available up to 15hp. (Offered in fully automatic and semi-automatic configurations)</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>images/MK Starter.jpg</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>lk_ea_products/brochures/Pump_Starter_and_Controller_Catalogue.pdf</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>Ensures safe operation across various conditions- offers high reliability; Can handle wide range of voltages from 200-400 V.; The design ensures reliable performance in adverse conditions such as hot, humid environments and supply voltage unbalance.; Built-in "ON &amp; OFF" indicators provide clear and immediate operational status to users.; Enhances durability and electrical conductivity for prolonged service life.; Rugged silver-tipped contacts enhance durability and electrical conductivity for prolonged service life.; The protective enclosure shields internal components from dust, humidity, and insects, enhancing longevity.</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>Thermal Overload Protection: Highly effective and reliable, ensuring safe operation under various conditions.; Field Proven Starters: Demonstrated reliability and effectiveness in real-world applications.; Wide Band Coil Operation: Capable of operating across a voltage range of 200-400 V.; Reliable Performance in Adverse Conditions: Ensures stable operation in hot, humid environments and under conditions of supply voltage unbalance.; Built-In “ON &amp; OFF” Indication: Provides clear status visibility to operators.; Protective Enclosure: Shields internal components from dust, humidity, and insects.; Compatibility with Voltage/Current Auto SPPR: Ensures seamless integration with safety and performance monitoring systems.; Connection Capability: Can be linked to a Dry Run Protection device to prevent operation under unsafe conditions.</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>https://www.lk-ea.com/products/pump-starters-and-controllers/controller/mr-gi-digital-single-phase-controller</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Lauritz Knudsen</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Electrical Equipment</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Downloaded</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Downloaded</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>MR-Gi Digital Single Phase Controller</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Controller</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>Since 1960, Lauritz Knudsen Electrical &amp; Automation has been integral to Indian agriculture and industry, offering a range of low voltage motor protection solutions. These systems ensure reliable and efficient irrigation and water management, supporting the daily needs of farmers and businesses Designed and developed in-house, our starters and controllers are the preferred choice for efficiently managing pump operations, saving both energy and time for our customers Available for both three-phase and single-phase applications, LK controllers not only protect the motor but also enhance convenience and safety for the user Featuring a robust contactor, Single Phase Preventer, and Dual Voltmeter &amp; Ammeter, this controller offers ease of installation, configuration, and maintenance. Seamlessly integrate it with communicable devices such as the M-POWER+ / M-POWER PRO / M-POWER++ modules for effortless remote pump operation Designed for up to 75 HP pumps in three-phase applications, our controllers efficiently operate agricultural motors and provide reliable protection. They offer overload protection, safeguard against phase unbalance, single phasing, and phase reversal failures, and include an auto-reset feature</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>The Digital single-phase controller is offered in three distinct variants to cater to a range of needs: MR-Gi, MR-GiA, and MR-GiB. The MR-Gi model is the manual version, designed for users who prefer control over the basic functions of their system. On the other hand, the MR-GiA and MR-GiB are equipped with automatic functionalities, enhancing convenience and efficiency. The MR-GiA variant is particularly advanced, featuring an in-built Water Level Controller (WLC) that automates water management. In contrast, the MR-GiB does not include a WLC, offering a simpler automatic option for users who do not require this feature. All variants are equipped with an automatic load setting and a digital display that provides critical real-time data on various operational parameters such as voltage and current. This feature allows for better monitoring and management of the controller's performance, ensuring optimal functionality and helping to prevent issues related to electrical parameters. Whether for residential, commercial, or agricultural use, each controller variant is designed to offer tailored solutions, ensuring users have the right tools for efficient management of their single-phase systems. Range Available: ﻿ 0.5 HP to 3 HP (Single Phase Applications Only)</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>images/MR-Gi Digital Single Phase Controller.jpg</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>lk_ea_products/brochures/MRGi_Controller_Catalogue.pdf</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>Manual mode provides direct control over the system, allowing users to adjust settings based on immediate needs or changes in conditions.; It enables operators to engage directly with the system, offering opportunities for hands-on troubleshooting and fine-tuning.; Automatic mode simplifies operations by managing routine tasks through pre-set controls, reducing the need for constant human intervention.; It enhances consistency in operations by maintaining optimal conditions automatically, minimizing the risk of human error.; Features like the inbuilt Water Level Controller automate water management, ensuring efficient use of resources and prevention of issues such as overflows or dry running.; Timers and delay functions in automatic mode help maintain a schedule, protect equipment, and conserve energy by running the system only when necessary.</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>Features: MR-Gi Manual version; Microcontroller Based Solution: Ensures precise control and monitoring.; Complete Protection: Guards against dry run, under-voltage, and over-voltage.; Current and Voltage Metering: Allows for detailed monitoring of electrical parameters.; Bypass Mode: Enables manual operation of the system.; Off Timer: Can controls the operational duration.; Digital Display: Provides real-time feedback on system status.; Automatic Current Setting: Adjusts electrical current automatically.; Capacitor Cut-off: Extends the life of capacitors.; Water Tank Status Indication: Indicates water level status to prevent overfill or depletion.</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>https://www.lk-ea.com/products/pump-starters-and-controllers/solar-solutions/solar-drive-controller</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Lauritz Knudsen</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Electrical Equipment</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Downloaded</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Downloaded</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Solar Drive Controller</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Solar Solutions</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>Lauritz Knudsen offers cutting-edge solar solutions with its Solar Drive Controller (Px3000), designed to power three-phase Submersible and Monoblock Pumps/Motors for a variety of applications, including irrigation, water supply, farm tank filling, and industrial activities. This robust controller features true MPPT (Maximum Power Point Tracking) to optimise performance even under cloudy conditions, ensuring maximum power extraction from PV panels. It automatically adjusts to changes in current and voltage to maximise output. With its dual supply capability, the Px3000 can operate on both solar and grid power, providing cost savings during daylight hours. Capable of handling input DC voltages up to 850V and operating at temperatures up to 50 degrees Celsius without derating, this controller sets the standard for reliability and efficiency in solar-powered water management</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>The Solar Drive Controller (Px3000) offers a robust and intuitive solution tailored to enhance the performance of three-phase submersible and monoblock pump motors across a wide range of applications, including irrigation, water supply, tank filling, and various industrial activities. Featuring advanced true Maximum Power Point Tracking (MPPT) technology, the Px3000 is engineered to optimize the efficiency of solar energy conversion, ensuring that pumps operate at peak performance even under varying solar conditions. Its plug-and-play design simplifies installation, allowing for immediate operation without the need for extensive setup. In addition to its powerful MPPT capability, the Px3000 is adept at functioning in less than ideal solar conditions, such as cloudy weather, ensuring that the maximum possible power is extracted from the photovoltaic (PV) panels at all times. This auto-adjustable feature dynamically alters current and voltage parameters to maximize output, enhancing overall energy efficiency. The dual supply capability of the controller allows it to switch seamlessly between solar and grid power, providing cost-effective operation by leveraging solar power during daylight hours. Furthermore, the controller's ability to operate at temperatures up to 50 degrees Celsius without any derating exemplifies its suitability for challenging environments, ensuring reliable performance regardless of external conditions. Range Available:</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>images/Solar Drive Controller.jpg</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>lk_ea_products/brochures/Px3000_Solar_Drive_Catalogues.pdf</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>True MPPT technology ensures that you get the most efficient use of solar energy throughout the day, maximising water output and reducing energy waste.; The controller's ability to automatically start and stop the pump based on sunlight intensity optimises energy use and prolongs the lifespan of the pump.; Dual energy compatibility provides the flexibility to switch between solar and grid power, ensuring reliable operation regardless of weather conditions and reducing dependency on non-renewable energy sources.; Reverse polarity protection safeguards the motor from installation errors, enhancing the system's reliability and reducing the risk of damage due to incorrect wiring.; The plug and play feature eliminates the need for manual parameter configuration, facilitating quick and easy setup that saves time and minimises setup errors.; A robust design capable of handling high input voltages up to 850V ensures the system can cope with variable solar intensities and maintain stable operation under diverse environmental conditions.</t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>True MPPT Technology: Maximizes water output during the day by optimally converting solar energy into usable power.; Automatic Operation: Automatically starts and stops the pump based on the intensity of sunlight, enhancing energy efficiency.; Dual Energy Compatibility: Operates seamlessly using either solar power or grid electricity, offering flexibility in energy sourcing.; Reverse Polarity Protection: Equipped with a feature that allows the motor to run correctly even if the PV wires are connected to opposite polarity terminals, preventing potential damage.; Plug &amp; Play Installation: Simplifies setup with easy installation; automatically detects and sets necessary parameters like Vmp and Voc without manual input.; Robust Design: Capable of handling very high input DC voltages up to 850V, making it suitable for a wide range of solar applications.</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>https://www.lk-ea.com/products/industrial-signalling-products/time-switches/astro</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Lauritz Knudsen</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Electrical Equipment</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Downloaded</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Downloaded</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Astro</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Time Switches</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>Time Switches are used for fixed time daily / weekly applications. They are ideal for lighting applications and also used to control air-conditioners / coolers, geysers, conveyers, pumps and exhaust fans etc.</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>An Astronomical Time Switch adjusts switching times automatically based on sunrise and sunset data for your location. It eliminates the need for seasonal reprogramming, making it ideal for outdoor lighting, signage, and security systems that require consistent operation year-round.</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>images/Astro.jpg</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>lk_ea_products/brochures/Panel_Accessories_Catalogue.pdf</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>https://www.lk-ea.com/products/industrial-signalling-products/push-buttons-indicating-lamps/gen-next-pro-22.5-mm</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Lauritz Knudsen</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Electrical Equipment</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Downloaded</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Downloaded</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
           <t>Gen next pro 22.5 mm</t>
         </is>
       </c>
-      <c r="H50" t="inlineStr">
+      <c r="H55" t="inlineStr">
         <is>
           <t>Push Buttons Indicating Lamps</t>
         </is>
       </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>Lauritz Knudsen Electrical &amp; Automation push buttons &amp; indicating lamps actuator is a cutting-edge solution designed for precise control and signaling in industrial environments. It prioritises safety without compromising functionality.</t>
-        </is>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>The 22mmGen Next Pro indicator integrates cutting-edge SMDCluster technology for superior illumination. It features inbuilt low voltage glow protection, ensuring accurate readings by preventing false indications due to stray voltages. This indicator is designed to pass stringent surge tests, making it a reliable choice for diverse panel applications.</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr"/>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>Bright and uniform illumination for clear visibility.; Withstands voltage fluctuations for reliable performance.; Endures harsh conditions for long-lasting durability.; Fits various panel installations for versatile application</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr">
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>Remote control units play a crucial role on factory shop floor for operational safety and reliability. Reliable push buttons and indicators have been trusted by users across industries for over 4 decades.</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>The 22.5mm Indicator is a panel-mounted visual device used to display the operational status of electrical circuits. Its larger size ensures high visibility, making it ideal for industrial control panels. Available in multiple colors, it supports quick status identification and enhances safety.</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
         <is>
           <t>images/Gen next pro 22.5 mm.jpg</t>
         </is>
       </c>
-      <c r="N50" t="inlineStr">
+      <c r="L55" t="inlineStr">
         <is>
           <t>lk_ea_products/brochures/Panel_Accessories_Catalogue.pdf</t>
         </is>
       </c>
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>https://www.lk-ea.com/products/industrial-signalling-products/push-buttons-indicating-lamps/gen-next-pro-16-mm</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Lauritz Knudsen</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Electrical Equipment</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Downloaded</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Downloaded</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Gen next pro 16 mm</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Push Buttons Indicating Lamps</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Remote control units play a crucial role on factory shop floor for operational safety and reliability. Reliable push buttons and indicators have been trusted by users across industries for over 4 decades.</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>The 16mm Indicator is a compact signaling device designed for space-constrained panels and enclosures. Despite its small footprint, it offers clear visual indication of circuit status. Suitable for instrumentation, control systems, and compact machinery.</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>images/Gen next pro 16 mm.jpg</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>lk_ea_products/brochures/Panel_Accessories_Catalogue.pdf</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>https://www.lk-ea.com/products/industrial-signalling-products/push-buttons-indicating-lamps/push-button-metal</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Lauritz Knudsen</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Electrical Equipment</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Downloaded</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Downloaded</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Push button metal</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Push Buttons Indicating Lamps</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>Remote control units play a crucial role on factory shop floor for operational safety and reliability. Reliable push buttons and indicators have been trusted by users across industries for over 4 decades.</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>Metal Push Buttons provide a rugged and durable interface for demanding environments. Offered in illuminated and non-illuminated types, they combine strength with functionality. Ideal for industrial machinery, outdoor panels, and high-usage areas.</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>images/Push button metal.jpg</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>lk_ea_products/brochures/Panel_Accessories_Catalogue.pdf</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>https://www.lk-ea.com/products/industrial-signalling-products/push-buttons-indicating-lamps/buzzer</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Lauritz Knudsen</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Electrical Equipment</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Downloaded</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Downloaded</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Buzzer</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Push Buttons Indicating Lamps</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>Remote control units play a crucial role on factory shop floor for operational safety and reliability. Reliable push buttons and indicators have been trusted by users across industries for over 4 decades.</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>The Buzzer is an audible alert device used to signal warnings, faults, or operational status. It produces a clear sound output, ensuring quick attention in control panels and alarm systems. Suitable for safety circuits and monitoring applications.</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>images/Buzzer.jpg</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>lk_ea_products/brochures/Panel_Accessories_Catalogue.pdf</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr"/>
+      <c r="N58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>https://www.lk-ea.com/products/industrial-signalling-products/push-buttons-indicating-lamps/push-button-stations</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Lauritz Knudsen</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Electrical Equipment</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Downloaded</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Downloaded</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Push button stations</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Push Buttons Indicating Lamps</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Remote control units play a crucial role on factory shop floor for operational safety and reliability. Reliable push buttons and indicators have been trusted by users across industries for over 4 decades.</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>A Push Button Station is a pre-assembled unit housing one or more push buttons for manual control. It simplifies installation and operation for start/stop and emergency functions. Commonly used in industrial setups, machinery, and process control systems</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>images/Push button stations.jpg</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>lk_ea_products/brochures/Panel_Accessories_Catalogue.pdf</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr"/>
+      <c r="N59" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>